<commit_message>
updates to modelling and checks
</commit_message>
<xml_diff>
--- a/Apps/head_to_head.xlsx
+++ b/Apps/head_to_head.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">start_time</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t xml:space="preserve">Midasbet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neds</t>
   </si>
   <si>
     <t xml:space="preserve">Playup</t>
@@ -562,16 +559,16 @@
         <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>5.085</v>
+        <v>4.61</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="n">
-        <v>1.209</v>
+        <v>1.228</v>
       </c>
       <c r="I2" t="n">
-        <v>2.379</v>
+        <v>3.125</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -594,16 +591,16 @@
         <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>5.085</v>
+        <v>4.61</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="n">
-        <v>1.1995</v>
+        <v>1.2185</v>
       </c>
       <c r="I3" t="n">
-        <v>3.034</v>
+        <v>3.76</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -626,16 +623,16 @@
         <v>13</v>
       </c>
       <c r="F4" t="n">
-        <v>5.085</v>
+        <v>4.61</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="n">
-        <v>1.19</v>
+        <v>1.209</v>
       </c>
       <c r="I4" t="n">
-        <v>3.699</v>
+        <v>4.405</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -658,16 +655,16 @@
         <v>13</v>
       </c>
       <c r="F5" t="n">
-        <v>4.7</v>
+        <v>4.75</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="I5" t="n">
-        <v>6.022</v>
+        <v>5.086</v>
       </c>
       <c r="J5" t="s">
         <v>16</v>
@@ -722,16 +719,16 @@
         <v>13</v>
       </c>
       <c r="F7" t="n">
-        <v>4.85</v>
+        <v>4.5</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="n">
-        <v>1.18</v>
+        <v>1.2</v>
       </c>
       <c r="I7" t="n">
-        <v>5.364</v>
+        <v>5.556</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -754,16 +751,16 @@
         <v>13</v>
       </c>
       <c r="F8" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="I8" t="n">
-        <v>6.485</v>
+        <v>6.256</v>
       </c>
       <c r="J8" t="s">
         <v>19</v>
@@ -786,16 +783,16 @@
         <v>13</v>
       </c>
       <c r="F9" t="n">
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="I9" t="n">
-        <v>5.086</v>
+        <v>5.556</v>
       </c>
       <c r="J9" t="s">
         <v>20</v>
@@ -818,16 +815,16 @@
         <v>13</v>
       </c>
       <c r="F10" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="I10" t="n">
-        <v>5.31</v>
+        <v>5.072</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -850,16 +847,16 @@
         <v>13</v>
       </c>
       <c r="F11" t="n">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="I11" t="n">
-        <v>5.556</v>
+        <v>5.31</v>
       </c>
       <c r="J11" t="s">
         <v>22</v>
@@ -882,16 +879,16 @@
         <v>13</v>
       </c>
       <c r="F12" t="n">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="I12" t="n">
-        <v>5.31</v>
+        <v>5.556</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
@@ -914,16 +911,16 @@
         <v>13</v>
       </c>
       <c r="F13" t="n">
-        <v>4.8</v>
+        <v>4.35</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>1.18</v>
+        <v>1.2</v>
       </c>
       <c r="I13" t="n">
-        <v>5.579</v>
+        <v>6.322</v>
       </c>
       <c r="J13" t="s">
         <v>24</v>
@@ -946,16 +943,16 @@
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>4.6</v>
+        <v>4.9</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>1.18</v>
+        <v>1.17857142857143</v>
       </c>
       <c r="I14" t="n">
-        <v>6.485</v>
+        <v>5.257</v>
       </c>
       <c r="J14" t="s">
         <v>25</v>
@@ -963,7 +960,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -972,25 +969,25 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F15" t="n">
-        <v>5.1</v>
+        <v>1.5985</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H15" t="n">
-        <v>1.16949152542373</v>
+        <v>2.425</v>
       </c>
       <c r="I15" t="n">
-        <v>5.115</v>
+        <v>3.796</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -1004,22 +1001,22 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="n">
+        <v>1.589</v>
+      </c>
+      <c r="G16" t="s">
         <v>28</v>
       </c>
-      <c r="F16" t="n">
-        <v>1.5795</v>
-      </c>
-      <c r="G16" t="s">
-        <v>29</v>
-      </c>
       <c r="H16" t="n">
-        <v>2.52</v>
+        <v>2.425</v>
       </c>
       <c r="I16" t="n">
-        <v>2.994</v>
+        <v>4.17</v>
       </c>
       <c r="J16" t="s">
         <v>15</v>
@@ -1036,22 +1033,22 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="n">
+        <v>1.5795</v>
+      </c>
+      <c r="G17" t="s">
         <v>28</v>
       </c>
-      <c r="F17" t="n">
-        <v>1.4845</v>
-      </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
       <c r="H17" t="n">
-        <v>2.52</v>
+        <v>2.425</v>
       </c>
       <c r="I17" t="n">
-        <v>7.045</v>
+        <v>4.548</v>
       </c>
       <c r="J17" t="s">
         <v>15</v>
@@ -1068,22 +1065,22 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
         <v>27</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
       </c>
       <c r="F18" t="n">
         <v>1.55</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" t="n">
-        <v>2.44</v>
+        <v>2.45</v>
       </c>
       <c r="I18" t="n">
-        <v>5.5</v>
+        <v>5.332</v>
       </c>
       <c r="J18" t="s">
         <v>16</v>
@@ -1100,16 +1097,16 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
         <v>27</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
       </c>
       <c r="F19" t="n">
         <v>1.58</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" t="n">
         <v>2.38</v>
@@ -1132,22 +1129,22 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="G20" t="s">
         <v>28</v>
       </c>
-      <c r="F20" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="G20" t="s">
-        <v>29</v>
-      </c>
       <c r="H20" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="I20" t="n">
-        <v>5.359</v>
+        <v>5.361</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
@@ -1164,22 +1161,22 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="G21" t="s">
         <v>28</v>
       </c>
-      <c r="F21" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="G21" t="s">
-        <v>29</v>
-      </c>
       <c r="H21" t="n">
-        <v>2.38</v>
+        <v>2.36</v>
       </c>
       <c r="I21" t="n">
-        <v>6.533</v>
+        <v>6.067</v>
       </c>
       <c r="J21" t="s">
         <v>19</v>
@@ -1196,22 +1193,22 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="G22" t="s">
         <v>28</v>
       </c>
-      <c r="F22" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
       <c r="H22" t="n">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="I22" t="n">
-        <v>4.511</v>
+        <v>4.958</v>
       </c>
       <c r="J22" t="s">
         <v>20</v>
@@ -1228,16 +1225,16 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
         <v>27</v>
-      </c>
-      <c r="E23" t="s">
-        <v>28</v>
       </c>
       <c r="F23" t="n">
         <v>1.55</v>
       </c>
       <c r="G23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" t="n">
         <v>2.45</v>
@@ -1260,22 +1257,22 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
         <v>27</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="G24" t="s">
         <v>28</v>
       </c>
-      <c r="F24" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
       <c r="H24" t="n">
-        <v>2.45</v>
+        <v>2.38</v>
       </c>
       <c r="I24" t="n">
-        <v>5.332</v>
+        <v>4.91</v>
       </c>
       <c r="J24" t="s">
         <v>22</v>
@@ -1292,16 +1289,16 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
         <v>27</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
       </c>
       <c r="F25" t="n">
         <v>1.58</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H25" t="n">
         <v>2.4</v>
@@ -1324,22 +1321,22 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
         <v>27</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="G26" t="s">
         <v>28</v>
       </c>
-      <c r="F26" t="n">
-        <v>1.58</v>
-      </c>
-      <c r="G26" t="s">
-        <v>29</v>
-      </c>
       <c r="H26" t="n">
-        <v>2.4</v>
+        <v>2.36</v>
       </c>
       <c r="I26" t="n">
-        <v>4.958</v>
+        <v>6.475</v>
       </c>
       <c r="J26" t="s">
         <v>24</v>
@@ -1356,22 +1353,22 @@
         <v>11</v>
       </c>
       <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
         <v>27</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="n">
+        <v>1.53763440860215</v>
+      </c>
+      <c r="G27" t="s">
         <v>28</v>
       </c>
-      <c r="F27" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="G27" t="s">
-        <v>29</v>
-      </c>
       <c r="H27" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I27" t="n">
-        <v>6.183</v>
+        <v>5.035</v>
       </c>
       <c r="J27" t="s">
         <v>25</v>
@@ -1388,25 +1385,25 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>1.53763440860215</v>
+        <v>3.5175</v>
       </c>
       <c r="G28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H28" t="n">
-        <v>2.5</v>
+        <v>1.3515</v>
       </c>
       <c r="I28" t="n">
-        <v>5.035</v>
+        <v>2.421</v>
       </c>
       <c r="J28" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -1420,22 +1417,22 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
         <v>30</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="n">
+        <v>3.5175</v>
+      </c>
+      <c r="G29" t="s">
         <v>31</v>
       </c>
-      <c r="F29" t="n">
-        <v>3.375</v>
-      </c>
-      <c r="G29" t="s">
-        <v>32</v>
-      </c>
       <c r="H29" t="n">
-        <v>1.266</v>
+        <v>1.342</v>
       </c>
       <c r="I29" t="n">
-        <v>8.619</v>
+        <v>2.945</v>
       </c>
       <c r="J29" t="s">
         <v>15</v>
@@ -1452,22 +1449,22 @@
         <v>11</v>
       </c>
       <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
         <v>30</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="n">
+        <v>3.5175</v>
+      </c>
+      <c r="G30" t="s">
         <v>31</v>
       </c>
-      <c r="F30" t="n">
-        <v>3.375</v>
-      </c>
-      <c r="G30" t="s">
-        <v>32</v>
-      </c>
       <c r="H30" t="n">
-        <v>1.2565</v>
+        <v>1.3325</v>
       </c>
       <c r="I30" t="n">
-        <v>9.216</v>
+        <v>3.476</v>
       </c>
       <c r="J30" t="s">
         <v>15</v>
@@ -1484,25 +1481,25 @@
         <v>11</v>
       </c>
       <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="n">
+        <v>3.4225</v>
+      </c>
+      <c r="G31" t="s">
         <v>31</v>
       </c>
-      <c r="F31" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="G31" t="s">
-        <v>32</v>
-      </c>
       <c r="H31" t="n">
-        <v>1.33</v>
+        <v>1.3515</v>
       </c>
       <c r="I31" t="n">
-        <v>5.491</v>
+        <v>3.21</v>
       </c>
       <c r="J31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
@@ -1516,25 +1513,25 @@
         <v>11</v>
       </c>
       <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="n">
+        <v>3.4225</v>
+      </c>
+      <c r="G32" t="s">
         <v>31</v>
       </c>
-      <c r="F32" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="G32" t="s">
-        <v>32</v>
-      </c>
       <c r="H32" t="n">
-        <v>1.33</v>
+        <v>1.342</v>
       </c>
       <c r="I32" t="n">
-        <v>5.039</v>
+        <v>3.734</v>
       </c>
       <c r="J32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
@@ -1548,25 +1545,25 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
         <v>30</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="n">
+        <v>3.4225</v>
+      </c>
+      <c r="G33" t="s">
         <v>31</v>
       </c>
-      <c r="F33" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="G33" t="s">
-        <v>32</v>
-      </c>
       <c r="H33" t="n">
-        <v>1.35</v>
+        <v>1.3325</v>
       </c>
       <c r="I33" t="n">
-        <v>5.324</v>
+        <v>4.265</v>
       </c>
       <c r="J33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
@@ -1580,25 +1577,25 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
         <v>30</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="G34" t="s">
         <v>31</v>
-      </c>
-      <c r="F34" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="G34" t="s">
-        <v>32</v>
       </c>
       <c r="H34" t="n">
         <v>1.32</v>
       </c>
       <c r="I34" t="n">
-        <v>6.527</v>
+        <v>5.169</v>
       </c>
       <c r="J34" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35">
@@ -1612,25 +1609,25 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
         <v>30</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="G35" t="s">
         <v>31</v>
       </c>
-      <c r="F35" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="G35" t="s">
-        <v>32</v>
-      </c>
       <c r="H35" t="n">
-        <v>1.35</v>
+        <v>1.33</v>
       </c>
       <c r="I35" t="n">
-        <v>4.843</v>
+        <v>5.039</v>
       </c>
       <c r="J35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36">
@@ -1644,25 +1641,25 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s">
         <v>30</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G36" t="s">
         <v>31</v>
       </c>
-      <c r="F36" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="G36" t="s">
-        <v>32</v>
-      </c>
       <c r="H36" t="n">
-        <v>1.34</v>
+        <v>1.3</v>
       </c>
       <c r="I36" t="n">
-        <v>5.396</v>
+        <v>5.495</v>
       </c>
       <c r="J36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
@@ -1676,25 +1673,25 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
         <v>30</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="G37" t="s">
         <v>31</v>
       </c>
-      <c r="F37" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>32</v>
-      </c>
       <c r="H37" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="I37" t="n">
-        <v>5.495</v>
+        <v>6.505</v>
       </c>
       <c r="J37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38">
@@ -1708,25 +1705,25 @@
         <v>11</v>
       </c>
       <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" t="s">
         <v>30</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="G38" t="s">
         <v>31</v>
       </c>
-      <c r="F38" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="G38" t="s">
-        <v>32</v>
-      </c>
       <c r="H38" t="n">
-        <v>1.33</v>
+        <v>1.29</v>
       </c>
       <c r="I38" t="n">
-        <v>4.862</v>
+        <v>5.297</v>
       </c>
       <c r="J38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
@@ -1740,25 +1737,25 @@
         <v>11</v>
       </c>
       <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
         <v>30</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="G39" t="s">
         <v>31</v>
       </c>
-      <c r="F39" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="G39" t="s">
-        <v>32</v>
-      </c>
       <c r="H39" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="I39" t="n">
-        <v>5.169</v>
+        <v>5.957</v>
       </c>
       <c r="J39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40">
@@ -1772,25 +1769,25 @@
         <v>11</v>
       </c>
       <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" t="s">
         <v>30</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="G40" t="s">
         <v>31</v>
       </c>
-      <c r="F40" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="G40" t="s">
-        <v>32</v>
-      </c>
       <c r="H40" t="n">
-        <v>1.32</v>
+        <v>1.3</v>
       </c>
       <c r="I40" t="n">
-        <v>6.527</v>
+        <v>5.172</v>
       </c>
       <c r="J40" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
@@ -1804,30 +1801,30 @@
         <v>11</v>
       </c>
       <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" t="s">
         <v>30</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="G41" t="s">
         <v>31</v>
       </c>
-      <c r="F41" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="G41" t="s">
-        <v>32</v>
-      </c>
       <c r="H41" t="n">
-        <v>1.31746031746032</v>
+        <v>1.29</v>
       </c>
       <c r="I41" t="n">
-        <v>5.315</v>
+        <v>5.297</v>
       </c>
       <c r="J41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>45164.2743055556</v>
+        <v>45164.15625</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -1836,30 +1833,30 @@
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F42" t="n">
-        <v>1.2</v>
+        <v>3.4</v>
       </c>
       <c r="G42" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H42" t="n">
-        <v>4.4</v>
+        <v>1.3</v>
       </c>
       <c r="I42" t="n">
-        <v>6.061</v>
+        <v>6.335</v>
       </c>
       <c r="J42" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45164.2743055556</v>
+        <v>45164.15625</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -1868,25 +1865,25 @@
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E43" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F43" t="n">
-        <v>1.22</v>
+        <v>3.4</v>
       </c>
       <c r="G43" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H43" t="n">
-        <v>4.3</v>
+        <v>1.31746031746032</v>
       </c>
       <c r="I43" t="n">
-        <v>5.223</v>
+        <v>5.315</v>
       </c>
       <c r="J43" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
@@ -1900,25 +1897,25 @@
         <v>11</v>
       </c>
       <c r="D44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" t="s">
         <v>33</v>
-      </c>
-      <c r="E44" t="s">
-        <v>34</v>
       </c>
       <c r="F44" t="n">
         <v>1.22</v>
       </c>
       <c r="G44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H44" t="n">
-        <v>4.3</v>
+        <v>4.25</v>
       </c>
       <c r="I44" t="n">
-        <v>5.223</v>
+        <v>5.497</v>
       </c>
       <c r="J44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45">
@@ -1932,25 +1929,25 @@
         <v>11</v>
       </c>
       <c r="D45" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" t="s">
         <v>33</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="G45" t="s">
         <v>34</v>
       </c>
-      <c r="F45" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="G45" t="s">
-        <v>35</v>
-      </c>
       <c r="H45" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="I45" t="n">
-        <v>4.694</v>
+        <v>5.035</v>
       </c>
       <c r="J45" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46">
@@ -1964,25 +1961,25 @@
         <v>11</v>
       </c>
       <c r="D46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" t="s">
         <v>33</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G46" t="s">
         <v>34</v>
       </c>
-      <c r="F46" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="G46" t="s">
-        <v>35</v>
-      </c>
       <c r="H46" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="I46" t="n">
-        <v>5.223</v>
+        <v>5</v>
       </c>
       <c r="J46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47">
@@ -1996,25 +1993,25 @@
         <v>11</v>
       </c>
       <c r="D47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" t="s">
         <v>33</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="G47" t="s">
         <v>34</v>
       </c>
-      <c r="F47" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="G47" t="s">
-        <v>35</v>
-      </c>
       <c r="H47" t="n">
-        <v>4.5</v>
+        <v>4.1</v>
       </c>
       <c r="I47" t="n">
-        <v>5.556</v>
+        <v>5.035</v>
       </c>
       <c r="J47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48">
@@ -2028,25 +2025,25 @@
         <v>11</v>
       </c>
       <c r="D48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" t="s">
         <v>33</v>
       </c>
-      <c r="E48" t="s">
-        <v>36</v>
-      </c>
       <c r="F48" t="n">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
       <c r="G48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H48" t="n">
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
       <c r="I48" t="n">
-        <v>4.83</v>
+        <v>5.556</v>
       </c>
       <c r="J48" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49">
@@ -2060,25 +2057,25 @@
         <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F49" t="n">
-        <v>1.22</v>
+        <v>1.23</v>
       </c>
       <c r="G49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H49" t="n">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="I49" t="n">
-        <v>5.223</v>
+        <v>5.11</v>
       </c>
       <c r="J49" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50">
@@ -2092,30 +2089,30 @@
         <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E50" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="G50" t="s">
         <v>34</v>
       </c>
-      <c r="F50" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="G50" t="s">
-        <v>35</v>
-      </c>
       <c r="H50" t="n">
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="I50" t="n">
-        <v>6.454</v>
+        <v>5.035</v>
       </c>
       <c r="J50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>45164.3923611111</v>
+        <v>45164.2743055556</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -2124,25 +2121,25 @@
         <v>11</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E51" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F51" t="n">
-        <v>1.7885</v>
+        <v>1.22</v>
       </c>
       <c r="G51" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H51" t="n">
-        <v>1.95</v>
+        <v>4.1</v>
       </c>
       <c r="I51" t="n">
-        <v>7.195</v>
+        <v>6.357</v>
       </c>
       <c r="J51" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52">
@@ -2156,22 +2153,22 @@
         <v>11</v>
       </c>
       <c r="D52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" t="s">
         <v>37</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="n">
+        <v>2.197</v>
+      </c>
+      <c r="G52" t="s">
         <v>38</v>
       </c>
-      <c r="F52" t="n">
-        <v>1.7885</v>
-      </c>
-      <c r="G52" t="s">
-        <v>39</v>
-      </c>
       <c r="H52" t="n">
-        <v>1.0095</v>
+        <v>1.703</v>
       </c>
       <c r="I52" t="n">
-        <v>54.972</v>
+        <v>4.237</v>
       </c>
       <c r="J52" t="s">
         <v>15</v>
@@ -2188,22 +2185,22 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" t="s">
         <v>37</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="n">
+        <v>2.197</v>
+      </c>
+      <c r="G53" t="s">
         <v>38</v>
       </c>
-      <c r="F53" t="n">
-        <v>1.779</v>
-      </c>
-      <c r="G53" t="s">
-        <v>39</v>
-      </c>
       <c r="H53" t="n">
-        <v>1.95</v>
+        <v>1.6935</v>
       </c>
       <c r="I53" t="n">
-        <v>7.493</v>
+        <v>4.566</v>
       </c>
       <c r="J53" t="s">
         <v>15</v>
@@ -2220,22 +2217,22 @@
         <v>11</v>
       </c>
       <c r="D54" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" t="s">
         <v>37</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="n">
+        <v>2.197</v>
+      </c>
+      <c r="G54" t="s">
         <v>38</v>
       </c>
-      <c r="F54" t="n">
-        <v>1.779</v>
-      </c>
-      <c r="G54" t="s">
-        <v>39</v>
-      </c>
       <c r="H54" t="n">
-        <v>1.0095</v>
+        <v>1.684</v>
       </c>
       <c r="I54" t="n">
-        <v>55.27</v>
+        <v>4.899</v>
       </c>
       <c r="J54" t="s">
         <v>15</v>
@@ -2252,25 +2249,25 @@
         <v>11</v>
       </c>
       <c r="D55" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" t="s">
         <v>37</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="G55" t="s">
         <v>38</v>
       </c>
-      <c r="F55" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="G55" t="s">
-        <v>39</v>
-      </c>
       <c r="H55" t="n">
-        <v>2.05</v>
+        <v>1.703</v>
       </c>
       <c r="I55" t="n">
-        <v>5.278</v>
+        <v>5.449</v>
       </c>
       <c r="J55" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56">
@@ -2284,25 +2281,25 @@
         <v>11</v>
       </c>
       <c r="D56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" t="s">
         <v>37</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="G56" t="s">
         <v>38</v>
       </c>
-      <c r="F56" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G56" t="s">
-        <v>39</v>
-      </c>
       <c r="H56" t="n">
-        <v>2</v>
+        <v>1.6935</v>
       </c>
       <c r="I56" t="n">
-        <v>5.556</v>
+        <v>5.778</v>
       </c>
       <c r="J56" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57">
@@ -2316,25 +2313,25 @@
         <v>11</v>
       </c>
       <c r="D57" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" t="s">
         <v>37</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="G57" t="s">
         <v>38</v>
       </c>
-      <c r="F57" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="G57" t="s">
-        <v>39</v>
-      </c>
       <c r="H57" t="n">
-        <v>2</v>
+        <v>1.684</v>
       </c>
       <c r="I57" t="n">
-        <v>6.497</v>
+        <v>6.111</v>
       </c>
       <c r="J57" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58">
@@ -2348,25 +2345,25 @@
         <v>11</v>
       </c>
       <c r="D58" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" t="s">
         <v>37</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="n">
+        <v>2.121</v>
+      </c>
+      <c r="G58" t="s">
         <v>38</v>
       </c>
-      <c r="F58" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="G58" t="s">
-        <v>39</v>
-      </c>
       <c r="H58" t="n">
-        <v>2.3</v>
+        <v>1.703</v>
       </c>
       <c r="I58" t="n">
-        <v>5.207</v>
+        <v>5.867</v>
       </c>
       <c r="J58" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59">
@@ -2380,25 +2377,25 @@
         <v>11</v>
       </c>
       <c r="D59" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" t="s">
         <v>37</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="n">
+        <v>2.121</v>
+      </c>
+      <c r="G59" t="s">
         <v>38</v>
       </c>
-      <c r="F59" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="G59" t="s">
-        <v>39</v>
-      </c>
       <c r="H59" t="n">
-        <v>2.05</v>
+        <v>1.6935</v>
       </c>
       <c r="I59" t="n">
-        <v>5.278</v>
+        <v>6.197</v>
       </c>
       <c r="J59" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60">
@@ -2412,25 +2409,25 @@
         <v>11</v>
       </c>
       <c r="D60" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" t="s">
         <v>37</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="n">
+        <v>2.121</v>
+      </c>
+      <c r="G60" t="s">
         <v>38</v>
       </c>
-      <c r="F60" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="G60" t="s">
-        <v>39</v>
-      </c>
       <c r="H60" t="n">
-        <v>2.1</v>
+        <v>1.684</v>
       </c>
       <c r="I60" t="n">
-        <v>5.423</v>
+        <v>6.53</v>
       </c>
       <c r="J60" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61">
@@ -2444,25 +2441,25 @@
         <v>11</v>
       </c>
       <c r="D61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" t="s">
         <v>37</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G61" t="s">
         <v>38</v>
       </c>
-      <c r="F61" t="n">
-        <v>1.77</v>
-      </c>
-      <c r="G61" t="s">
-        <v>39</v>
-      </c>
       <c r="H61" t="n">
-        <v>2.1</v>
+        <v>1.67</v>
       </c>
       <c r="I61" t="n">
-        <v>4.116</v>
+        <v>5.335</v>
       </c>
       <c r="J61" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62">
@@ -2476,25 +2473,25 @@
         <v>11</v>
       </c>
       <c r="D62" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" t="s">
         <v>37</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="G62" t="s">
         <v>38</v>
       </c>
-      <c r="F62" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G62" t="s">
-        <v>40</v>
-      </c>
       <c r="H62" t="n">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="I62" t="n">
-        <v>5.556</v>
+        <v>5.335</v>
       </c>
       <c r="J62" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63">
@@ -2508,25 +2505,25 @@
         <v>11</v>
       </c>
       <c r="D63" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" t="s">
         <v>37</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="G63" t="s">
         <v>38</v>
       </c>
-      <c r="F63" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G63" t="s">
-        <v>39</v>
-      </c>
       <c r="H63" t="n">
-        <v>1.96</v>
+        <v>1.7</v>
       </c>
       <c r="I63" t="n">
-        <v>6.576</v>
+        <v>5.335</v>
       </c>
       <c r="J63" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64">
@@ -2540,30 +2537,30 @@
         <v>11</v>
       </c>
       <c r="D64" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" t="s">
         <v>37</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G64" t="s">
         <v>38</v>
       </c>
-      <c r="F64" t="n">
-        <v>1.77519379844961</v>
-      </c>
-      <c r="G64" t="s">
-        <v>39</v>
-      </c>
       <c r="H64" t="n">
-        <v>2.05</v>
+        <v>1.7</v>
       </c>
       <c r="I64" t="n">
-        <v>5.112</v>
+        <v>6.443</v>
       </c>
       <c r="J64" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45164.4236111111</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
@@ -2572,30 +2569,30 @@
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E65" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F65" t="n">
-        <v>5.275</v>
+        <v>2.1</v>
       </c>
       <c r="G65" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H65" t="n">
-        <v>1.1995</v>
+        <v>1.74</v>
       </c>
       <c r="I65" t="n">
-        <v>2.325</v>
+        <v>5.09</v>
       </c>
       <c r="J65" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45164.4236111111</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -2604,30 +2601,30 @@
         <v>11</v>
       </c>
       <c r="D66" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E66" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F66" t="n">
-        <v>5.275</v>
+        <v>2.1</v>
       </c>
       <c r="G66" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H66" t="n">
-        <v>1.19</v>
+        <v>1.73</v>
       </c>
       <c r="I66" t="n">
-        <v>2.991</v>
+        <v>5.423</v>
       </c>
       <c r="J66" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45164.4236111111</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -2636,30 +2633,30 @@
         <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E67" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F67" t="n">
-        <v>5.275</v>
+        <v>2.13</v>
       </c>
       <c r="G67" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H67" t="n">
-        <v>1.1805</v>
+        <v>1.72</v>
       </c>
       <c r="I67" t="n">
-        <v>3.667</v>
+        <v>5.088</v>
       </c>
       <c r="J67" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45164.4236111111</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -2668,30 +2665,30 @@
         <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E68" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F68" t="n">
-        <v>4.895</v>
+        <v>2.1</v>
       </c>
       <c r="G68" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H68" t="n">
-        <v>1.1995</v>
+        <v>1.74</v>
       </c>
       <c r="I68" t="n">
-        <v>3.797</v>
+        <v>5.09</v>
       </c>
       <c r="J68" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45164.4236111111</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -2700,30 +2697,30 @@
         <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E69" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F69" t="n">
-        <v>4.895</v>
+        <v>2.08</v>
       </c>
       <c r="G69" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H69" t="n">
-        <v>1.19</v>
+        <v>1.7</v>
       </c>
       <c r="I69" t="n">
-        <v>4.463</v>
+        <v>6.9</v>
       </c>
       <c r="J69" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45164.4236111111</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -2732,25 +2729,25 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E70" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F70" t="n">
-        <v>4.895</v>
+        <v>2.1</v>
       </c>
       <c r="G70" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H70" t="n">
-        <v>1.1805</v>
+        <v>1.73529411764706</v>
       </c>
       <c r="I70" t="n">
-        <v>5.139</v>
+        <v>5.246</v>
       </c>
       <c r="J70" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71">
@@ -2764,25 +2761,25 @@
         <v>11</v>
       </c>
       <c r="D71" t="s">
+        <v>40</v>
+      </c>
+      <c r="E71" t="s">
         <v>41</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="n">
+        <v>5.085</v>
+      </c>
+      <c r="G71" t="s">
         <v>42</v>
       </c>
-      <c r="F71" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="G71" t="s">
-        <v>43</v>
-      </c>
       <c r="H71" t="n">
-        <v>1.15</v>
+        <v>1.2185</v>
       </c>
       <c r="I71" t="n">
-        <v>6.564</v>
+        <v>1.734</v>
       </c>
       <c r="J71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72">
@@ -2796,25 +2793,25 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" t="s">
         <v>41</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="n">
+        <v>5.085</v>
+      </c>
+      <c r="G72" t="s">
         <v>42</v>
       </c>
-      <c r="F72" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="G72" t="s">
-        <v>43</v>
-      </c>
       <c r="H72" t="n">
-        <v>1.2</v>
+        <v>1.209</v>
       </c>
       <c r="I72" t="n">
-        <v>5.072</v>
+        <v>2.379</v>
       </c>
       <c r="J72" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73">
@@ -2828,25 +2825,25 @@
         <v>11</v>
       </c>
       <c r="D73" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" t="s">
         <v>41</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="n">
+        <v>5.085</v>
+      </c>
+      <c r="G73" t="s">
         <v>42</v>
       </c>
-      <c r="F73" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G73" t="s">
-        <v>43</v>
-      </c>
       <c r="H73" t="n">
-        <v>1.18</v>
+        <v>1.1995</v>
       </c>
       <c r="I73" t="n">
-        <v>5.579</v>
+        <v>3.034</v>
       </c>
       <c r="J73" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74">
@@ -2860,25 +2857,25 @@
         <v>11</v>
       </c>
       <c r="D74" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" t="s">
         <v>41</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="n">
+        <v>5</v>
+      </c>
+      <c r="G74" t="s">
         <v>42</v>
       </c>
-      <c r="F74" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G74" t="s">
-        <v>43</v>
-      </c>
       <c r="H74" t="n">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
       <c r="I74" t="n">
-        <v>6.256</v>
+        <v>5.47</v>
       </c>
       <c r="J74" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75">
@@ -2892,25 +2889,25 @@
         <v>11</v>
       </c>
       <c r="D75" t="s">
+        <v>40</v>
+      </c>
+      <c r="E75" t="s">
         <v>41</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G75" t="s">
         <v>42</v>
       </c>
-      <c r="F75" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="G75" t="s">
-        <v>43</v>
-      </c>
       <c r="H75" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="I75" t="n">
-        <v>4.701</v>
+        <v>5.072</v>
       </c>
       <c r="J75" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76">
@@ -2924,25 +2921,25 @@
         <v>11</v>
       </c>
       <c r="D76" t="s">
+        <v>40</v>
+      </c>
+      <c r="E76" t="s">
         <v>41</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G76" t="s">
         <v>42</v>
       </c>
-      <c r="F76" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="G76" t="s">
-        <v>43</v>
-      </c>
       <c r="H76" t="n">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="I76" t="n">
-        <v>5.072</v>
+        <v>5.579</v>
       </c>
       <c r="J76" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77">
@@ -2956,25 +2953,25 @@
         <v>11</v>
       </c>
       <c r="D77" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" t="s">
         <v>41</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G77" t="s">
         <v>42</v>
       </c>
-      <c r="F77" t="n">
-        <v>5</v>
-      </c>
-      <c r="G77" t="s">
-        <v>43</v>
-      </c>
       <c r="H77" t="n">
-        <v>1.17</v>
+        <v>1.18</v>
       </c>
       <c r="I77" t="n">
-        <v>5.47</v>
+        <v>6.485</v>
       </c>
       <c r="J77" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78">
@@ -2988,25 +2985,25 @@
         <v>11</v>
       </c>
       <c r="D78" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" t="s">
         <v>41</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G78" t="s">
         <v>42</v>
-      </c>
-      <c r="F78" t="n">
-        <v>4.45</v>
-      </c>
-      <c r="G78" t="s">
-        <v>43</v>
       </c>
       <c r="H78" t="n">
         <v>1.2</v>
       </c>
       <c r="I78" t="n">
-        <v>5.805</v>
+        <v>5.556</v>
       </c>
       <c r="J78" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79">
@@ -3020,25 +3017,25 @@
         <v>11</v>
       </c>
       <c r="D79" t="s">
+        <v>40</v>
+      </c>
+      <c r="E79" t="s">
         <v>41</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F79" t="n">
+        <v>5</v>
+      </c>
+      <c r="G79" t="s">
         <v>42</v>
       </c>
-      <c r="F79" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G79" t="s">
-        <v>43</v>
-      </c>
       <c r="H79" t="n">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
       <c r="I79" t="n">
-        <v>5.556</v>
+        <v>5.47</v>
       </c>
       <c r="J79" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80">
@@ -3052,30 +3049,30 @@
         <v>11</v>
       </c>
       <c r="D80" t="s">
+        <v>40</v>
+      </c>
+      <c r="E80" t="s">
         <v>41</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F80" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="G80" t="s">
         <v>42</v>
       </c>
-      <c r="F80" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="G80" t="s">
-        <v>43</v>
-      </c>
       <c r="H80" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="I80" t="n">
-        <v>5.072</v>
+        <v>5.086</v>
       </c>
       <c r="J80" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>45165.1041666667</v>
+        <v>45164.4236111111</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
@@ -3084,30 +3081,30 @@
         <v>11</v>
       </c>
       <c r="D81" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E81" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F81" t="n">
-        <v>1.1235</v>
+        <v>4.5</v>
       </c>
       <c r="G81" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H81" t="n">
-        <v>6.51</v>
+        <v>1.2</v>
       </c>
       <c r="I81" t="n">
-        <v>4.369</v>
+        <v>5.556</v>
       </c>
       <c r="J81" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>45165.1041666667</v>
+        <v>45164.4236111111</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
@@ -3116,25 +3113,25 @@
         <v>11</v>
       </c>
       <c r="D82" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F82" t="n">
-        <v>1.114</v>
+        <v>4.75</v>
       </c>
       <c r="G82" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H82" t="n">
-        <v>6.51</v>
+        <v>1.18867924528302</v>
       </c>
       <c r="I82" t="n">
-        <v>5.128</v>
+        <v>5.18</v>
       </c>
       <c r="J82" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83">
@@ -3148,22 +3145,22 @@
         <v>11</v>
       </c>
       <c r="D83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" t="s">
         <v>44</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="n">
+        <v>1.133</v>
+      </c>
+      <c r="G83" t="s">
         <v>45</v>
       </c>
-      <c r="F83" t="n">
-        <v>1.1045</v>
-      </c>
-      <c r="G83" t="s">
-        <v>46</v>
-      </c>
       <c r="H83" t="n">
-        <v>6.51</v>
+        <v>5.655</v>
       </c>
       <c r="I83" t="n">
-        <v>5.9</v>
+        <v>5.945</v>
       </c>
       <c r="J83" t="s">
         <v>15</v>
@@ -3180,25 +3177,25 @@
         <v>11</v>
       </c>
       <c r="D84" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" t="s">
         <v>44</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="n">
+        <v>1.1235</v>
+      </c>
+      <c r="G84" t="s">
         <v>45</v>
       </c>
-      <c r="F84" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G84" t="s">
-        <v>46</v>
-      </c>
       <c r="H84" t="n">
-        <v>6</v>
+        <v>5.655</v>
       </c>
       <c r="I84" t="n">
-        <v>5.952</v>
+        <v>6.691</v>
       </c>
       <c r="J84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85">
@@ -3212,25 +3209,25 @@
         <v>11</v>
       </c>
       <c r="D85" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" t="s">
         <v>44</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F85" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G85" t="s">
         <v>45</v>
       </c>
-      <c r="F85" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G85" t="s">
-        <v>46</v>
-      </c>
       <c r="H85" t="n">
-        <v>6.25</v>
+        <v>6.5</v>
       </c>
       <c r="I85" t="n">
-        <v>5.286</v>
+        <v>5.475</v>
       </c>
       <c r="J85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86">
@@ -3244,25 +3241,25 @@
         <v>11</v>
       </c>
       <c r="D86" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" t="s">
         <v>44</v>
-      </c>
-      <c r="E86" t="s">
-        <v>45</v>
       </c>
       <c r="F86" t="n">
         <v>1.12</v>
       </c>
       <c r="G86" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H86" t="n">
-        <v>6.2</v>
+        <v>6.25</v>
       </c>
       <c r="I86" t="n">
-        <v>5.415</v>
+        <v>5.286</v>
       </c>
       <c r="J86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87">
@@ -3276,25 +3273,25 @@
         <v>11</v>
       </c>
       <c r="D87" t="s">
+        <v>43</v>
+      </c>
+      <c r="E87" t="s">
         <v>44</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G87" t="s">
         <v>45</v>
       </c>
-      <c r="F87" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G87" t="s">
-        <v>46</v>
-      </c>
       <c r="H87" t="n">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="I87" t="n">
-        <v>6.757</v>
+        <v>5.415</v>
       </c>
       <c r="J87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88">
@@ -3308,25 +3305,25 @@
         <v>11</v>
       </c>
       <c r="D88" t="s">
+        <v>43</v>
+      </c>
+      <c r="E88" t="s">
         <v>44</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G88" t="s">
         <v>45</v>
       </c>
-      <c r="F88" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G88" t="s">
-        <v>46</v>
-      </c>
       <c r="H88" t="n">
-        <v>6.2</v>
+        <v>5.9</v>
       </c>
       <c r="I88" t="n">
-        <v>4.625</v>
+        <v>7.039</v>
       </c>
       <c r="J88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89">
@@ -3340,25 +3337,25 @@
         <v>11</v>
       </c>
       <c r="D89" t="s">
+        <v>43</v>
+      </c>
+      <c r="E89" t="s">
         <v>44</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G89" t="s">
         <v>45</v>
       </c>
-      <c r="F89" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G89" t="s">
-        <v>46</v>
-      </c>
       <c r="H89" t="n">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="I89" t="n">
-        <v>5.162</v>
+        <v>5.475</v>
       </c>
       <c r="J89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90">
@@ -3372,16 +3369,16 @@
         <v>11</v>
       </c>
       <c r="D90" t="s">
+        <v>43</v>
+      </c>
+      <c r="E90" t="s">
         <v>44</v>
-      </c>
-      <c r="E90" t="s">
-        <v>45</v>
       </c>
       <c r="F90" t="n">
         <v>1.12</v>
       </c>
       <c r="G90" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H90" t="n">
         <v>6.25</v>
@@ -3390,7 +3387,7 @@
         <v>5.286</v>
       </c>
       <c r="J90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91">
@@ -3404,16 +3401,16 @@
         <v>11</v>
       </c>
       <c r="D91" t="s">
+        <v>43</v>
+      </c>
+      <c r="E91" t="s">
         <v>44</v>
-      </c>
-      <c r="E91" t="s">
-        <v>45</v>
       </c>
       <c r="F91" t="n">
         <v>1.13</v>
       </c>
       <c r="G91" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H91" t="n">
         <v>6.05</v>
@@ -3422,7 +3419,7 @@
         <v>5.025</v>
       </c>
       <c r="J91" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92">
@@ -3436,25 +3433,25 @@
         <v>11</v>
       </c>
       <c r="D92" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" t="s">
         <v>44</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G92" t="s">
         <v>45</v>
       </c>
-      <c r="F92" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G92" t="s">
-        <v>46</v>
-      </c>
       <c r="H92" t="n">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="I92" t="n">
-        <v>5.415</v>
+        <v>5.475</v>
       </c>
       <c r="J92" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93">
@@ -3468,25 +3465,25 @@
         <v>11</v>
       </c>
       <c r="D93" t="s">
+        <v>43</v>
+      </c>
+      <c r="E93" t="s">
         <v>44</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G93" t="s">
         <v>45</v>
-      </c>
-      <c r="F93" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G93" t="s">
-        <v>46</v>
       </c>
       <c r="H93" t="n">
         <v>6</v>
       </c>
       <c r="I93" t="n">
-        <v>6.757</v>
+        <v>5.952</v>
       </c>
       <c r="J93" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94">
@@ -3500,16 +3497,16 @@
         <v>11</v>
       </c>
       <c r="D94" t="s">
+        <v>43</v>
+      </c>
+      <c r="E94" t="s">
         <v>44</v>
-      </c>
-      <c r="E94" t="s">
-        <v>45</v>
       </c>
       <c r="F94" t="n">
         <v>1.11976047904192</v>
       </c>
       <c r="G94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H94" t="n">
         <v>6.25</v>
@@ -3518,7 +3515,7 @@
         <v>5.305</v>
       </c>
       <c r="J94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95">
@@ -3532,25 +3529,25 @@
         <v>11</v>
       </c>
       <c r="D95" t="s">
+        <v>46</v>
+      </c>
+      <c r="E95" t="s">
         <v>47</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G95" t="s">
         <v>48</v>
       </c>
-      <c r="F95" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="G95" t="s">
-        <v>49</v>
-      </c>
       <c r="H95" t="n">
-        <v>2.064</v>
+        <v>2</v>
       </c>
       <c r="I95" t="n">
-        <v>5.268</v>
+        <v>5.556</v>
       </c>
       <c r="J95" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96">
@@ -3564,25 +3561,25 @@
         <v>11</v>
       </c>
       <c r="D96" t="s">
+        <v>46</v>
+      </c>
+      <c r="E96" t="s">
         <v>47</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G96" t="s">
         <v>48</v>
       </c>
-      <c r="F96" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="G96" t="s">
-        <v>49</v>
-      </c>
       <c r="H96" t="n">
-        <v>1.95</v>
+        <v>2.02</v>
       </c>
       <c r="I96" t="n">
-        <v>8.1</v>
+        <v>5.061</v>
       </c>
       <c r="J96" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97">
@@ -3596,25 +3593,25 @@
         <v>11</v>
       </c>
       <c r="D97" t="s">
+        <v>46</v>
+      </c>
+      <c r="E97" t="s">
         <v>47</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F97" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G97" t="s">
         <v>48</v>
       </c>
-      <c r="F97" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="G97" t="s">
-        <v>49</v>
-      </c>
       <c r="H97" t="n">
-        <v>1.7885</v>
+        <v>2</v>
       </c>
       <c r="I97" t="n">
-        <v>12.731</v>
+        <v>5.556</v>
       </c>
       <c r="J97" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98">
@@ -3628,25 +3625,25 @@
         <v>11</v>
       </c>
       <c r="D98" t="s">
+        <v>46</v>
+      </c>
+      <c r="E98" t="s">
         <v>47</v>
       </c>
-      <c r="E98" t="s">
+      <c r="F98" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="G98" t="s">
         <v>48</v>
       </c>
-      <c r="F98" t="n">
-        <v>1.627</v>
-      </c>
-      <c r="G98" t="s">
-        <v>49</v>
-      </c>
       <c r="H98" t="n">
-        <v>2.064</v>
+        <v>2</v>
       </c>
       <c r="I98" t="n">
-        <v>9.912</v>
+        <v>6.18</v>
       </c>
       <c r="J98" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="99">
@@ -3660,25 +3657,25 @@
         <v>11</v>
       </c>
       <c r="D99" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" t="s">
         <v>47</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G99" t="s">
         <v>48</v>
       </c>
-      <c r="F99" t="n">
-        <v>1.627</v>
-      </c>
-      <c r="G99" t="s">
-        <v>49</v>
-      </c>
       <c r="H99" t="n">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="I99" t="n">
-        <v>12.745</v>
+        <v>5.556</v>
       </c>
       <c r="J99" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100">
@@ -3692,25 +3689,25 @@
         <v>11</v>
       </c>
       <c r="D100" t="s">
+        <v>46</v>
+      </c>
+      <c r="E100" t="s">
         <v>47</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G100" t="s">
         <v>48</v>
       </c>
-      <c r="F100" t="n">
-        <v>1.627</v>
-      </c>
-      <c r="G100" t="s">
-        <v>49</v>
-      </c>
       <c r="H100" t="n">
-        <v>1.7885</v>
+        <v>2.08</v>
       </c>
       <c r="I100" t="n">
-        <v>17.376</v>
+        <v>5.22</v>
       </c>
       <c r="J100" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101">
@@ -3724,25 +3721,25 @@
         <v>11</v>
       </c>
       <c r="D101" t="s">
+        <v>46</v>
+      </c>
+      <c r="E101" t="s">
         <v>47</v>
-      </c>
-      <c r="E101" t="s">
-        <v>48</v>
       </c>
       <c r="F101" t="n">
         <v>1.81</v>
       </c>
       <c r="G101" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H101" t="n">
-        <v>2</v>
+        <v>2.04</v>
       </c>
       <c r="I101" t="n">
-        <v>5.249</v>
+        <v>4.268</v>
       </c>
       <c r="J101" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102">
@@ -3756,25 +3753,25 @@
         <v>11</v>
       </c>
       <c r="D102" t="s">
+        <v>46</v>
+      </c>
+      <c r="E102" t="s">
         <v>47</v>
-      </c>
-      <c r="E102" t="s">
-        <v>48</v>
       </c>
       <c r="F102" t="n">
         <v>1.8</v>
       </c>
       <c r="G102" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H102" t="n">
-        <v>2.02</v>
+        <v>2</v>
       </c>
       <c r="I102" t="n">
-        <v>5.061</v>
+        <v>5.556</v>
       </c>
       <c r="J102" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103">
@@ -3788,25 +3785,25 @@
         <v>11</v>
       </c>
       <c r="D103" t="s">
+        <v>46</v>
+      </c>
+      <c r="E103" t="s">
         <v>47</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="G103" t="s">
         <v>48</v>
-      </c>
-      <c r="F103" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G103" t="s">
-        <v>49</v>
       </c>
       <c r="H103" t="n">
         <v>2</v>
       </c>
       <c r="I103" t="n">
-        <v>5.556</v>
+        <v>6.18</v>
       </c>
       <c r="J103" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104">
@@ -3820,30 +3817,30 @@
         <v>11</v>
       </c>
       <c r="D104" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104" t="s">
         <v>47</v>
       </c>
-      <c r="E104" t="s">
+      <c r="F104" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G104" t="s">
         <v>48</v>
       </c>
-      <c r="F104" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="G104" t="s">
-        <v>49</v>
-      </c>
       <c r="H104" t="n">
-        <v>1.98</v>
+        <v>2.02</v>
       </c>
       <c r="I104" t="n">
-        <v>6.371</v>
+        <v>5.061</v>
       </c>
       <c r="J104" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
@@ -3852,30 +3849,30 @@
         <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E105" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F105" t="n">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G105" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H105" t="n">
-        <v>2.02</v>
+        <v>2.6</v>
       </c>
       <c r="I105" t="n">
-        <v>5.061</v>
+        <v>5.128</v>
       </c>
       <c r="J105" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B106" t="s">
         <v>10</v>
@@ -3884,30 +3881,30 @@
         <v>11</v>
       </c>
       <c r="D106" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E106" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F106" t="n">
-        <v>1.8</v>
+        <v>1.52</v>
       </c>
       <c r="G106" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H106" t="n">
-        <v>2</v>
+        <v>2.55</v>
       </c>
       <c r="I106" t="n">
-        <v>5.556</v>
+        <v>5.005</v>
       </c>
       <c r="J106" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B107" t="s">
         <v>10</v>
@@ -3916,30 +3913,30 @@
         <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E107" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F107" t="n">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="G107" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H107" t="n">
-        <v>2.08</v>
+        <v>2.6</v>
       </c>
       <c r="I107" t="n">
-        <v>5.22</v>
+        <v>5.128</v>
       </c>
       <c r="J107" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B108" t="s">
         <v>10</v>
@@ -3948,30 +3945,30 @@
         <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E108" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F108" t="n">
-        <v>1.81</v>
+        <v>1.5</v>
       </c>
       <c r="G108" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H108" t="n">
-        <v>2.04</v>
+        <v>2.5</v>
       </c>
       <c r="I108" t="n">
-        <v>4.268</v>
+        <v>6.667</v>
       </c>
       <c r="J108" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B109" t="s">
         <v>10</v>
@@ -3980,30 +3977,30 @@
         <v>11</v>
       </c>
       <c r="D109" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E109" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F109" t="n">
-        <v>1.8</v>
+        <v>1.53</v>
       </c>
       <c r="G109" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H109" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I109" t="n">
-        <v>5.556</v>
+        <v>5.359</v>
       </c>
       <c r="J109" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B110" t="s">
         <v>10</v>
@@ -4012,30 +4009,30 @@
         <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E110" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F110" t="n">
-        <v>1.8</v>
+        <v>1.52</v>
       </c>
       <c r="G110" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H110" t="n">
-        <v>1.96</v>
+        <v>2.54</v>
       </c>
       <c r="I110" t="n">
-        <v>6.576</v>
+        <v>5.16</v>
       </c>
       <c r="J110" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.3402777778</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -4044,25 +4041,25 @@
         <v>11</v>
       </c>
       <c r="D111" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E111" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F111" t="n">
-        <v>1.8</v>
+        <v>1.52</v>
       </c>
       <c r="G111" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H111" t="n">
-        <v>2.02</v>
+        <v>2.55</v>
       </c>
       <c r="I111" t="n">
-        <v>5.061</v>
+        <v>5.005</v>
       </c>
       <c r="J111" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112">
@@ -4076,25 +4073,25 @@
         <v>11</v>
       </c>
       <c r="D112" t="s">
+        <v>49</v>
+      </c>
+      <c r="E112" t="s">
         <v>50</v>
       </c>
-      <c r="E112" t="s">
+      <c r="F112" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G112" t="s">
         <v>51</v>
       </c>
-      <c r="F112" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="G112" t="s">
-        <v>52</v>
-      </c>
       <c r="H112" t="n">
-        <v>2.65</v>
+        <v>2.5</v>
       </c>
       <c r="I112" t="n">
-        <v>6.229</v>
+        <v>6.667</v>
       </c>
       <c r="J112" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113">
@@ -4108,281 +4105,25 @@
         <v>11</v>
       </c>
       <c r="D113" t="s">
+        <v>49</v>
+      </c>
+      <c r="E113" t="s">
         <v>50</v>
       </c>
-      <c r="E113" t="s">
+      <c r="F113" t="n">
+        <v>1.51282051282051</v>
+      </c>
+      <c r="G113" t="s">
         <v>51</v>
       </c>
-      <c r="F113" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G113" t="s">
-        <v>52</v>
-      </c>
       <c r="H113" t="n">
-        <v>2.6</v>
+        <v>2.55</v>
       </c>
       <c r="I113" t="n">
-        <v>5.128</v>
+        <v>5.317</v>
       </c>
       <c r="J113" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B114" t="s">
-        <v>10</v>
-      </c>
-      <c r="C114" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114" t="s">
-        <v>50</v>
-      </c>
-      <c r="E114" t="s">
-        <v>51</v>
-      </c>
-      <c r="F114" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="G114" t="s">
-        <v>52</v>
-      </c>
-      <c r="H114" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="I114" t="n">
-        <v>5.303</v>
-      </c>
-      <c r="J114" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B115" t="s">
-        <v>10</v>
-      </c>
-      <c r="C115" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" t="s">
-        <v>50</v>
-      </c>
-      <c r="E115" t="s">
-        <v>51</v>
-      </c>
-      <c r="F115" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="G115" t="s">
-        <v>52</v>
-      </c>
-      <c r="H115" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="I115" t="n">
-        <v>6.489</v>
-      </c>
-      <c r="J115" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B116" t="s">
-        <v>10</v>
-      </c>
-      <c r="C116" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" t="s">
-        <v>50</v>
-      </c>
-      <c r="E116" t="s">
-        <v>51</v>
-      </c>
-      <c r="F116" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="G116" t="s">
-        <v>52</v>
-      </c>
-      <c r="H116" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="I116" t="n">
-        <v>5.303</v>
-      </c>
-      <c r="J116" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B117" t="s">
-        <v>10</v>
-      </c>
-      <c r="C117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D117" t="s">
-        <v>50</v>
-      </c>
-      <c r="E117" t="s">
-        <v>51</v>
-      </c>
-      <c r="F117" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G117" t="s">
-        <v>52</v>
-      </c>
-      <c r="H117" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="I117" t="n">
-        <v>5.128</v>
-      </c>
-      <c r="J117" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B118" t="s">
-        <v>10</v>
-      </c>
-      <c r="C118" t="s">
-        <v>11</v>
-      </c>
-      <c r="D118" t="s">
-        <v>50</v>
-      </c>
-      <c r="E118" t="s">
-        <v>51</v>
-      </c>
-      <c r="F118" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="G118" t="s">
-        <v>52</v>
-      </c>
-      <c r="H118" t="n">
-        <v>2.69</v>
-      </c>
-      <c r="I118" t="n">
-        <v>5.202</v>
-      </c>
-      <c r="J118" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B119" t="s">
-        <v>10</v>
-      </c>
-      <c r="C119" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" t="s">
-        <v>50</v>
-      </c>
-      <c r="E119" t="s">
-        <v>51</v>
-      </c>
-      <c r="F119" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G119" t="s">
-        <v>53</v>
-      </c>
-      <c r="H119" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="I119" t="n">
-        <v>5.128</v>
-      </c>
-      <c r="J119" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B120" t="s">
-        <v>10</v>
-      </c>
-      <c r="C120" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" t="s">
-        <v>50</v>
-      </c>
-      <c r="E120" t="s">
-        <v>51</v>
-      </c>
-      <c r="F120" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="G120" t="s">
-        <v>52</v>
-      </c>
-      <c r="H120" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="I120" t="n">
-        <v>6.783</v>
-      </c>
-      <c r="J120" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>45165.3402777778</v>
-      </c>
-      <c r="B121" t="s">
-        <v>10</v>
-      </c>
-      <c r="C121" t="s">
-        <v>11</v>
-      </c>
-      <c r="D121" t="s">
-        <v>50</v>
-      </c>
-      <c r="E121" t="s">
-        <v>51</v>
-      </c>
-      <c r="F121" t="n">
-        <v>1.47619047619048</v>
-      </c>
-      <c r="G121" t="s">
-        <v>52</v>
-      </c>
-      <c r="H121" t="n">
-        <v>2.65</v>
-      </c>
-      <c r="I121" t="n">
-        <v>5.478</v>
-      </c>
-      <c r="J121" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all coaches votes 2023
</commit_message>
<xml_diff>
--- a/Apps/head_to_head.xlsx
+++ b/Apps/head_to_head.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">start_time</t>
   </si>
@@ -50,13 +50,13 @@
     <t xml:space="preserve">Round 24</t>
   </si>
   <si>
-    <t xml:space="preserve">Essendon v Collingwood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Essendon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collingwood</t>
+    <t xml:space="preserve">Hawthorn v Fremantle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawthorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fremantle</t>
   </si>
   <si>
     <t xml:space="preserve">Betfair</t>
@@ -74,6 +74,9 @@
     <t xml:space="preserve">Midasbet</t>
   </si>
   <si>
+    <t xml:space="preserve">Neds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Playup</t>
   </si>
   <si>
@@ -90,15 +93,6 @@
   </si>
   <si>
     <t xml:space="preserve">Unibet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hawthorn v Fremantle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hawthorn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fremantle</t>
   </si>
   <si>
     <t xml:space="preserve">North Melbourne v Gold Coast</t>
@@ -544,7 +538,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -559,16 +553,16 @@
         <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>4.61</v>
+        <v>1.703</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="n">
-        <v>1.228</v>
+        <v>2.273</v>
       </c>
       <c r="I2" t="n">
-        <v>3.125</v>
+        <v>2.715</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -576,7 +570,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -591,16 +585,16 @@
         <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>4.61</v>
+        <v>1.703</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="n">
-        <v>1.2185</v>
+        <v>2.254</v>
       </c>
       <c r="I3" t="n">
-        <v>3.76</v>
+        <v>3.085</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -608,7 +602,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -623,16 +617,16 @@
         <v>13</v>
       </c>
       <c r="F4" t="n">
-        <v>4.61</v>
+        <v>1.703</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="n">
-        <v>1.209</v>
+        <v>2.235</v>
       </c>
       <c r="I4" t="n">
-        <v>4.405</v>
+        <v>3.463</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -640,7 +634,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -655,24 +649,24 @@
         <v>13</v>
       </c>
       <c r="F5" t="n">
-        <v>4.75</v>
+        <v>1.6935</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="n">
-        <v>1.19</v>
+        <v>2.273</v>
       </c>
       <c r="I5" t="n">
-        <v>5.086</v>
+        <v>3.044</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -687,24 +681,24 @@
         <v>13</v>
       </c>
       <c r="F6" t="n">
-        <v>4.6</v>
+        <v>1.6935</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="n">
-        <v>1.2</v>
+        <v>2.254</v>
       </c>
       <c r="I6" t="n">
-        <v>5.072</v>
+        <v>3.415</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -719,24 +713,24 @@
         <v>13</v>
       </c>
       <c r="F7" t="n">
-        <v>4.5</v>
+        <v>1.6935</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="n">
-        <v>1.2</v>
+        <v>2.235</v>
       </c>
       <c r="I7" t="n">
-        <v>5.556</v>
+        <v>3.792</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -751,24 +745,24 @@
         <v>13</v>
       </c>
       <c r="F8" t="n">
-        <v>4.5</v>
+        <v>1.684</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="n">
-        <v>1.19</v>
+        <v>2.273</v>
       </c>
       <c r="I8" t="n">
-        <v>6.256</v>
+        <v>3.377</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -783,24 +777,24 @@
         <v>13</v>
       </c>
       <c r="F9" t="n">
-        <v>4.5</v>
+        <v>1.684</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="n">
-        <v>1.2</v>
+        <v>2.254</v>
       </c>
       <c r="I9" t="n">
-        <v>5.556</v>
+        <v>3.748</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -815,24 +809,24 @@
         <v>13</v>
       </c>
       <c r="F10" t="n">
-        <v>4.6</v>
+        <v>1.684</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="n">
-        <v>1.2</v>
+        <v>2.235</v>
       </c>
       <c r="I10" t="n">
-        <v>5.072</v>
+        <v>4.125</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -847,24 +841,24 @@
         <v>13</v>
       </c>
       <c r="F11" t="n">
-        <v>4.7</v>
+        <v>1.62</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="n">
-        <v>1.19</v>
+        <v>2.3</v>
       </c>
       <c r="I11" t="n">
-        <v>5.31</v>
+        <v>5.207</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -879,24 +873,24 @@
         <v>13</v>
       </c>
       <c r="F12" t="n">
-        <v>4.5</v>
+        <v>1.67</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="n">
-        <v>1.2</v>
+        <v>2.2</v>
       </c>
       <c r="I12" t="n">
-        <v>5.556</v>
+        <v>5.335</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -911,24 +905,24 @@
         <v>13</v>
       </c>
       <c r="F13" t="n">
-        <v>4.35</v>
+        <v>1.62</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>1.2</v>
+        <v>2.3</v>
       </c>
       <c r="I13" t="n">
-        <v>6.322</v>
+        <v>5.207</v>
       </c>
       <c r="J13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45163.4097222222</v>
+        <v>45164.15625</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -943,19 +937,19 @@
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>4.9</v>
+        <v>1.64</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>1.17857142857143</v>
+        <v>2.2</v>
       </c>
       <c r="I14" t="n">
-        <v>5.257</v>
+        <v>6.43</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -969,25 +963,25 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>1.5985</v>
+        <v>1.62</v>
       </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H15" t="n">
-        <v>2.425</v>
+        <v>2.3</v>
       </c>
       <c r="I15" t="n">
-        <v>3.796</v>
+        <v>5.207</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -1001,25 +995,25 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F16" t="n">
-        <v>1.589</v>
+        <v>1.62</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H16" t="n">
-        <v>2.425</v>
+        <v>2.3</v>
       </c>
       <c r="I16" t="n">
-        <v>4.17</v>
+        <v>5.207</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -1033,25 +1027,25 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>1.5795</v>
+        <v>1.65</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H17" t="n">
-        <v>2.425</v>
+        <v>2.3</v>
       </c>
       <c r="I17" t="n">
-        <v>4.548</v>
+        <v>4.084</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
@@ -1065,25 +1059,25 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F18" t="n">
-        <v>1.55</v>
+        <v>1.68</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H18" t="n">
-        <v>2.45</v>
+        <v>2.15</v>
       </c>
       <c r="I18" t="n">
-        <v>5.332</v>
+        <v>6.035</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
@@ -1097,25 +1091,25 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>1.58</v>
+        <v>1.65</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H19" t="n">
-        <v>2.38</v>
+        <v>2.25</v>
       </c>
       <c r="I19" t="n">
-        <v>5.308</v>
+        <v>5.051</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
@@ -1129,25 +1123,25 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F20" t="n">
-        <v>1.57</v>
+        <v>1.62</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H20" t="n">
-        <v>2.4</v>
+        <v>2.28</v>
       </c>
       <c r="I20" t="n">
-        <v>5.361</v>
+        <v>5.588</v>
       </c>
       <c r="J20" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -1161,25 +1155,25 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.61728395061728</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="I21" t="n">
+        <v>5.692</v>
+      </c>
+      <c r="J21" t="s">
         <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="G21" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" t="n">
-        <v>2.36</v>
-      </c>
-      <c r="I21" t="n">
-        <v>6.067</v>
-      </c>
-      <c r="J21" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -1193,25 +1187,25 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" t="n">
-        <v>1.58</v>
+        <v>4.895</v>
       </c>
       <c r="G22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H22" t="n">
-        <v>2.4</v>
+        <v>1.228</v>
       </c>
       <c r="I22" t="n">
-        <v>4.958</v>
+        <v>1.862</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
@@ -1225,25 +1219,25 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F23" t="n">
-        <v>1.55</v>
+        <v>4.895</v>
       </c>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H23" t="n">
-        <v>2.45</v>
+        <v>1.2185</v>
       </c>
       <c r="I23" t="n">
-        <v>5.332</v>
+        <v>2.497</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -1257,25 +1251,25 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F24" t="n">
-        <v>1.59</v>
+        <v>4.895</v>
       </c>
       <c r="G24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H24" t="n">
-        <v>2.38</v>
+        <v>1.209</v>
       </c>
       <c r="I24" t="n">
-        <v>4.91</v>
+        <v>3.142</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
@@ -1289,25 +1283,25 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F25" t="n">
-        <v>1.58</v>
+        <v>4.8</v>
       </c>
       <c r="G25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H25" t="n">
-        <v>2.4</v>
+        <v>1.228</v>
       </c>
       <c r="I25" t="n">
-        <v>4.958</v>
+        <v>2.267</v>
       </c>
       <c r="J25" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
@@ -1321,25 +1315,25 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F26" t="n">
-        <v>1.56</v>
+        <v>4.8</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H26" t="n">
-        <v>2.36</v>
+        <v>1.2185</v>
       </c>
       <c r="I26" t="n">
-        <v>6.475</v>
+        <v>2.901</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
@@ -1353,25 +1347,25 @@
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F27" t="n">
-        <v>1.53763440860215</v>
+        <v>4.8</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H27" t="n">
-        <v>2.5</v>
+        <v>1.209</v>
       </c>
       <c r="I27" t="n">
-        <v>5.035</v>
+        <v>3.546</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
@@ -1385,25 +1379,25 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G28" t="s">
         <v>29</v>
       </c>
-      <c r="E28" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" t="n">
-        <v>3.5175</v>
-      </c>
-      <c r="G28" t="s">
-        <v>31</v>
-      </c>
       <c r="H28" t="n">
-        <v>1.3515</v>
+        <v>1.2</v>
       </c>
       <c r="I28" t="n">
-        <v>2.421</v>
+        <v>5.556</v>
       </c>
       <c r="J28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29">
@@ -1417,25 +1411,25 @@
         <v>11</v>
       </c>
       <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="G29" t="s">
         <v>29</v>
       </c>
-      <c r="E29" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" t="n">
-        <v>3.5175</v>
-      </c>
-      <c r="G29" t="s">
-        <v>31</v>
-      </c>
       <c r="H29" t="n">
-        <v>1.342</v>
+        <v>1.23</v>
       </c>
       <c r="I29" t="n">
-        <v>2.945</v>
+        <v>4.83</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
@@ -1449,25 +1443,25 @@
         <v>11</v>
       </c>
       <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G30" t="s">
         <v>29</v>
       </c>
-      <c r="E30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" t="n">
-        <v>3.5175</v>
-      </c>
-      <c r="G30" t="s">
-        <v>31</v>
-      </c>
       <c r="H30" t="n">
-        <v>1.3325</v>
+        <v>1.21</v>
       </c>
       <c r="I30" t="n">
-        <v>3.476</v>
+        <v>5.372</v>
       </c>
       <c r="J30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
@@ -1481,25 +1475,25 @@
         <v>11</v>
       </c>
       <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G31" t="s">
         <v>29</v>
       </c>
-      <c r="E31" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" t="n">
-        <v>3.4225</v>
-      </c>
-      <c r="G31" t="s">
-        <v>31</v>
-      </c>
       <c r="H31" t="n">
-        <v>1.3515</v>
+        <v>1.22</v>
       </c>
       <c r="I31" t="n">
-        <v>3.21</v>
+        <v>6.357</v>
       </c>
       <c r="J31" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
@@ -1513,25 +1507,25 @@
         <v>11</v>
       </c>
       <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
         <v>29</v>
       </c>
-      <c r="E32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" t="n">
-        <v>3.4225</v>
-      </c>
-      <c r="G32" t="s">
-        <v>31</v>
-      </c>
       <c r="H32" t="n">
-        <v>1.342</v>
+        <v>1.25</v>
       </c>
       <c r="I32" t="n">
-        <v>3.734</v>
+        <v>5</v>
       </c>
       <c r="J32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
@@ -1545,25 +1539,25 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G33" t="s">
         <v>29</v>
       </c>
-      <c r="E33" t="s">
-        <v>30</v>
-      </c>
-      <c r="F33" t="n">
-        <v>3.4225</v>
-      </c>
-      <c r="G33" t="s">
-        <v>31</v>
-      </c>
       <c r="H33" t="n">
-        <v>1.3325</v>
+        <v>1.22</v>
       </c>
       <c r="I33" t="n">
-        <v>4.265</v>
+        <v>5.223</v>
       </c>
       <c r="J33" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34">
@@ -1577,25 +1571,25 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G34" t="s">
         <v>29</v>
       </c>
-      <c r="E34" t="s">
-        <v>30</v>
-      </c>
-      <c r="F34" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="G34" t="s">
-        <v>31</v>
-      </c>
       <c r="H34" t="n">
-        <v>1.32</v>
+        <v>1.2</v>
       </c>
       <c r="I34" t="n">
-        <v>5.169</v>
+        <v>5.072</v>
       </c>
       <c r="J34" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
@@ -1609,25 +1603,25 @@
         <v>11</v>
       </c>
       <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="G35" t="s">
         <v>29</v>
       </c>
-      <c r="E35" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="G35" t="s">
-        <v>31</v>
-      </c>
       <c r="H35" t="n">
-        <v>1.33</v>
+        <v>1.23</v>
       </c>
       <c r="I35" t="n">
-        <v>5.039</v>
+        <v>5.992</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36">
@@ -1641,25 +1635,25 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G36" t="s">
         <v>29</v>
       </c>
-      <c r="E36" t="s">
-        <v>30</v>
-      </c>
-      <c r="F36" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G36" t="s">
-        <v>31</v>
-      </c>
       <c r="H36" t="n">
-        <v>1.3</v>
+        <v>1.22</v>
       </c>
       <c r="I36" t="n">
-        <v>5.495</v>
+        <v>5.223</v>
       </c>
       <c r="J36" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37">
@@ -1673,25 +1667,25 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G37" t="s">
         <v>29</v>
       </c>
-      <c r="E37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="G37" t="s">
-        <v>31</v>
-      </c>
       <c r="H37" t="n">
-        <v>1.29</v>
+        <v>1.22</v>
       </c>
       <c r="I37" t="n">
-        <v>6.505</v>
+        <v>5.223</v>
       </c>
       <c r="J37" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
@@ -1705,30 +1699,30 @@
         <v>11</v>
       </c>
       <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="G38" t="s">
         <v>29</v>
       </c>
-      <c r="E38" t="s">
-        <v>30</v>
-      </c>
-      <c r="F38" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="G38" t="s">
-        <v>31</v>
-      </c>
       <c r="H38" t="n">
-        <v>1.29</v>
+        <v>1.21978021978022</v>
       </c>
       <c r="I38" t="n">
-        <v>5.297</v>
+        <v>5.511</v>
       </c>
       <c r="J38" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>45164.15625</v>
+        <v>45164.2743055556</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -1737,30 +1731,30 @@
         <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F39" t="n">
-        <v>3.25</v>
+        <v>1.22</v>
       </c>
       <c r="G39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H39" t="n">
-        <v>1.33</v>
+        <v>4.3</v>
       </c>
       <c r="I39" t="n">
-        <v>5.957</v>
+        <v>5.223</v>
       </c>
       <c r="J39" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>45164.15625</v>
+        <v>45164.2743055556</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
@@ -1769,30 +1763,30 @@
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F40" t="n">
-        <v>3.54</v>
+        <v>1.22</v>
       </c>
       <c r="G40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H40" t="n">
-        <v>1.3</v>
+        <v>4.3</v>
       </c>
       <c r="I40" t="n">
-        <v>5.172</v>
+        <v>5.223</v>
       </c>
       <c r="J40" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>45164.15625</v>
+        <v>45164.2743055556</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -1801,30 +1795,30 @@
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F41" t="n">
-        <v>3.6</v>
+        <v>1.23</v>
       </c>
       <c r="G41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H41" t="n">
-        <v>1.29</v>
+        <v>4.15</v>
       </c>
       <c r="I41" t="n">
-        <v>5.297</v>
+        <v>5.397</v>
       </c>
       <c r="J41" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>45164.15625</v>
+        <v>45164.2743055556</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
@@ -1833,30 +1827,30 @@
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F42" t="n">
-        <v>3.4</v>
+        <v>1.19</v>
       </c>
       <c r="G42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H42" t="n">
-        <v>1.3</v>
+        <v>4.6</v>
       </c>
       <c r="I42" t="n">
-        <v>6.335</v>
+        <v>5.773</v>
       </c>
       <c r="J42" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45164.15625</v>
+        <v>45164.2743055556</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
@@ -1865,25 +1859,25 @@
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F43" t="n">
-        <v>3.4</v>
+        <v>1.22</v>
       </c>
       <c r="G43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H43" t="n">
-        <v>1.31746031746032</v>
+        <v>4.3</v>
       </c>
       <c r="I43" t="n">
-        <v>5.315</v>
+        <v>5.223</v>
       </c>
       <c r="J43" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
@@ -1897,25 +1891,25 @@
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F44" t="n">
         <v>1.22</v>
       </c>
       <c r="G44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H44" t="n">
-        <v>4.25</v>
+        <v>4.3</v>
       </c>
       <c r="I44" t="n">
-        <v>5.497</v>
+        <v>5.223</v>
       </c>
       <c r="J44" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
@@ -1929,25 +1923,25 @@
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
         <v>33</v>
       </c>
       <c r="F45" t="n">
-        <v>1.24</v>
+        <v>1.17</v>
       </c>
       <c r="G45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H45" t="n">
-        <v>4.1</v>
+        <v>4.85</v>
       </c>
       <c r="I45" t="n">
-        <v>5.035</v>
+        <v>6.089</v>
       </c>
       <c r="J45" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46">
@@ -1961,25 +1955,25 @@
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
         <v>33</v>
       </c>
       <c r="F46" t="n">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="G46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H46" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="I46" t="n">
-        <v>5</v>
+        <v>5.556</v>
       </c>
       <c r="J46" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47">
@@ -1993,30 +1987,30 @@
         <v>11</v>
       </c>
       <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="G47" t="s">
         <v>32</v>
       </c>
-      <c r="E47" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47" t="n">
-        <v>1.24</v>
-      </c>
-      <c r="G47" t="s">
-        <v>34</v>
-      </c>
       <c r="H47" t="n">
-        <v>4.1</v>
+        <v>4.3</v>
       </c>
       <c r="I47" t="n">
-        <v>5.035</v>
+        <v>5.223</v>
       </c>
       <c r="J47" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>45164.2743055556</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
@@ -2025,30 +2019,30 @@
         <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F48" t="n">
-        <v>1.2</v>
+        <v>2.482</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H48" t="n">
-        <v>4.5</v>
+        <v>1.5985</v>
       </c>
       <c r="I48" t="n">
-        <v>5.556</v>
+        <v>2.849</v>
       </c>
       <c r="J48" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>45164.2743055556</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
@@ -2057,30 +2051,30 @@
         <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
         <v>35</v>
       </c>
       <c r="F49" t="n">
-        <v>1.23</v>
+        <v>2.482</v>
       </c>
       <c r="G49" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H49" t="n">
-        <v>4.2</v>
+        <v>1.589</v>
       </c>
       <c r="I49" t="n">
-        <v>5.11</v>
+        <v>3.223</v>
       </c>
       <c r="J49" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>45164.2743055556</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -2089,30 +2083,30 @@
         <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E50" t="s">
         <v>35</v>
       </c>
       <c r="F50" t="n">
-        <v>1.24</v>
+        <v>2.482</v>
       </c>
       <c r="G50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H50" t="n">
-        <v>4.1</v>
+        <v>1.5795</v>
       </c>
       <c r="I50" t="n">
-        <v>5.035</v>
+        <v>3.601</v>
       </c>
       <c r="J50" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>45164.2743055556</v>
+        <v>45164.3923611111</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -2121,25 +2115,25 @@
         <v>11</v>
       </c>
       <c r="D51" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F51" t="n">
-        <v>1.22</v>
+        <v>2.463</v>
       </c>
       <c r="G51" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H51" t="n">
-        <v>4.1</v>
+        <v>1.5985</v>
       </c>
       <c r="I51" t="n">
-        <v>6.357</v>
+        <v>3.16</v>
       </c>
       <c r="J51" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52">
@@ -2153,22 +2147,22 @@
         <v>11</v>
       </c>
       <c r="D52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2.463</v>
+      </c>
+      <c r="G52" t="s">
         <v>36</v>
       </c>
-      <c r="E52" t="s">
-        <v>37</v>
-      </c>
-      <c r="F52" t="n">
-        <v>2.197</v>
-      </c>
-      <c r="G52" t="s">
-        <v>38</v>
-      </c>
       <c r="H52" t="n">
-        <v>1.703</v>
+        <v>1.589</v>
       </c>
       <c r="I52" t="n">
-        <v>4.237</v>
+        <v>3.534</v>
       </c>
       <c r="J52" t="s">
         <v>15</v>
@@ -2185,22 +2179,22 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2.463</v>
+      </c>
+      <c r="G53" t="s">
         <v>36</v>
       </c>
-      <c r="E53" t="s">
-        <v>37</v>
-      </c>
-      <c r="F53" t="n">
-        <v>2.197</v>
-      </c>
-      <c r="G53" t="s">
-        <v>38</v>
-      </c>
       <c r="H53" t="n">
-        <v>1.6935</v>
+        <v>1.5795</v>
       </c>
       <c r="I53" t="n">
-        <v>4.566</v>
+        <v>3.912</v>
       </c>
       <c r="J53" t="s">
         <v>15</v>
@@ -2217,22 +2211,22 @@
         <v>11</v>
       </c>
       <c r="D54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F54" t="n">
+        <v>2.444</v>
+      </c>
+      <c r="G54" t="s">
         <v>36</v>
       </c>
-      <c r="E54" t="s">
-        <v>37</v>
-      </c>
-      <c r="F54" t="n">
-        <v>2.197</v>
-      </c>
-      <c r="G54" t="s">
-        <v>38</v>
-      </c>
       <c r="H54" t="n">
-        <v>1.684</v>
+        <v>1.5985</v>
       </c>
       <c r="I54" t="n">
-        <v>4.899</v>
+        <v>3.475</v>
       </c>
       <c r="J54" t="s">
         <v>15</v>
@@ -2249,22 +2243,22 @@
         <v>11</v>
       </c>
       <c r="D55" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2.444</v>
+      </c>
+      <c r="G55" t="s">
         <v>36</v>
       </c>
-      <c r="E55" t="s">
-        <v>37</v>
-      </c>
-      <c r="F55" t="n">
-        <v>2.14</v>
-      </c>
-      <c r="G55" t="s">
-        <v>38</v>
-      </c>
       <c r="H55" t="n">
-        <v>1.703</v>
+        <v>1.589</v>
       </c>
       <c r="I55" t="n">
-        <v>5.449</v>
+        <v>3.849</v>
       </c>
       <c r="J55" t="s">
         <v>15</v>
@@ -2281,22 +2275,22 @@
         <v>11</v>
       </c>
       <c r="D56" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" t="n">
+        <v>2.444</v>
+      </c>
+      <c r="G56" t="s">
         <v>36</v>
       </c>
-      <c r="E56" t="s">
-        <v>37</v>
-      </c>
-      <c r="F56" t="n">
-        <v>2.14</v>
-      </c>
-      <c r="G56" t="s">
-        <v>38</v>
-      </c>
       <c r="H56" t="n">
-        <v>1.6935</v>
+        <v>1.5795</v>
       </c>
       <c r="I56" t="n">
-        <v>5.778</v>
+        <v>4.228</v>
       </c>
       <c r="J56" t="s">
         <v>15</v>
@@ -2313,25 +2307,25 @@
         <v>11</v>
       </c>
       <c r="D57" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G57" t="s">
         <v>36</v>
       </c>
-      <c r="E57" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" t="n">
-        <v>2.14</v>
-      </c>
-      <c r="G57" t="s">
-        <v>38</v>
-      </c>
       <c r="H57" t="n">
-        <v>1.684</v>
+        <v>1.6</v>
       </c>
       <c r="I57" t="n">
-        <v>6.111</v>
+        <v>5.053</v>
       </c>
       <c r="J57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
@@ -2345,25 +2339,25 @@
         <v>11</v>
       </c>
       <c r="D58" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="G58" t="s">
         <v>36</v>
       </c>
-      <c r="E58" t="s">
-        <v>37</v>
-      </c>
-      <c r="F58" t="n">
-        <v>2.121</v>
-      </c>
-      <c r="G58" t="s">
-        <v>38</v>
-      </c>
       <c r="H58" t="n">
-        <v>1.703</v>
+        <v>1.56</v>
       </c>
       <c r="I58" t="n">
-        <v>5.867</v>
+        <v>5.425</v>
       </c>
       <c r="J58" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59">
@@ -2377,25 +2371,25 @@
         <v>11</v>
       </c>
       <c r="D59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" t="s">
-        <v>37</v>
-      </c>
-      <c r="F59" t="n">
-        <v>2.121</v>
-      </c>
-      <c r="G59" t="s">
-        <v>38</v>
-      </c>
       <c r="H59" t="n">
-        <v>1.6935</v>
+        <v>1.6</v>
       </c>
       <c r="I59" t="n">
-        <v>6.197</v>
+        <v>5.053</v>
       </c>
       <c r="J59" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60">
@@ -2409,25 +2403,25 @@
         <v>11</v>
       </c>
       <c r="D60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="G60" t="s">
         <v>36</v>
       </c>
-      <c r="E60" t="s">
-        <v>37</v>
-      </c>
-      <c r="F60" t="n">
-        <v>2.121</v>
-      </c>
-      <c r="G60" t="s">
-        <v>38</v>
-      </c>
       <c r="H60" t="n">
-        <v>1.684</v>
+        <v>1.56</v>
       </c>
       <c r="I60" t="n">
-        <v>6.53</v>
+        <v>6.119</v>
       </c>
       <c r="J60" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61">
@@ -2441,25 +2435,25 @@
         <v>11</v>
       </c>
       <c r="D61" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G61" t="s">
         <v>36</v>
       </c>
-      <c r="E61" t="s">
-        <v>37</v>
-      </c>
-      <c r="F61" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="G61" t="s">
-        <v>38</v>
-      </c>
       <c r="H61" t="n">
-        <v>1.67</v>
+        <v>1.6</v>
       </c>
       <c r="I61" t="n">
-        <v>5.335</v>
+        <v>5.053</v>
       </c>
       <c r="J61" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62">
@@ -2473,25 +2467,25 @@
         <v>11</v>
       </c>
       <c r="D62" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G62" t="s">
         <v>36</v>
       </c>
-      <c r="E62" t="s">
-        <v>37</v>
-      </c>
-      <c r="F62" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="G62" t="s">
-        <v>38</v>
-      </c>
       <c r="H62" t="n">
-        <v>1.7</v>
+        <v>1.55</v>
       </c>
       <c r="I62" t="n">
-        <v>5.335</v>
+        <v>5.332</v>
       </c>
       <c r="J62" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63">
@@ -2505,25 +2499,25 @@
         <v>11</v>
       </c>
       <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G63" t="s">
         <v>36</v>
       </c>
-      <c r="E63" t="s">
-        <v>37</v>
-      </c>
-      <c r="F63" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="G63" t="s">
-        <v>38</v>
-      </c>
       <c r="H63" t="n">
-        <v>1.7</v>
+        <v>1.57</v>
       </c>
       <c r="I63" t="n">
-        <v>5.335</v>
+        <v>5.361</v>
       </c>
       <c r="J63" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64">
@@ -2537,25 +2531,25 @@
         <v>11</v>
       </c>
       <c r="D64" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="G64" t="s">
         <v>36</v>
       </c>
-      <c r="E64" t="s">
-        <v>37</v>
-      </c>
-      <c r="F64" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="G64" t="s">
-        <v>38</v>
-      </c>
       <c r="H64" t="n">
-        <v>1.7</v>
+        <v>1.56</v>
       </c>
       <c r="I64" t="n">
-        <v>6.443</v>
+        <v>6.119</v>
       </c>
       <c r="J64" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65">
@@ -2569,25 +2563,25 @@
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E65" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G65" t="s">
         <v>37</v>
       </c>
-      <c r="F65" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="G65" t="s">
-        <v>38</v>
-      </c>
       <c r="H65" t="n">
-        <v>1.74</v>
+        <v>1.55</v>
       </c>
       <c r="I65" t="n">
-        <v>5.09</v>
+        <v>5.332</v>
       </c>
       <c r="J65" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66">
@@ -2601,25 +2595,25 @@
         <v>11</v>
       </c>
       <c r="D66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G66" t="s">
         <v>36</v>
       </c>
-      <c r="E66" t="s">
-        <v>37</v>
-      </c>
-      <c r="F66" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="G66" t="s">
-        <v>38</v>
-      </c>
       <c r="H66" t="n">
-        <v>1.73</v>
+        <v>1.57</v>
       </c>
       <c r="I66" t="n">
-        <v>5.423</v>
+        <v>5.361</v>
       </c>
       <c r="J66" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67">
@@ -2633,30 +2627,30 @@
         <v>11</v>
       </c>
       <c r="D67" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G67" t="s">
         <v>36</v>
       </c>
-      <c r="E67" t="s">
-        <v>37</v>
-      </c>
-      <c r="F67" t="n">
-        <v>2.13</v>
-      </c>
-      <c r="G67" t="s">
-        <v>38</v>
-      </c>
       <c r="H67" t="n">
-        <v>1.72</v>
+        <v>1.57142857142857</v>
       </c>
       <c r="I67" t="n">
-        <v>5.088</v>
+        <v>5.303</v>
       </c>
       <c r="J67" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45164.3923611111</v>
+        <v>45164.4236111111</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -2665,30 +2659,30 @@
         <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E68" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F68" t="n">
-        <v>2.1</v>
+        <v>4.705</v>
       </c>
       <c r="G68" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H68" t="n">
-        <v>1.74</v>
+        <v>1.228</v>
       </c>
       <c r="I68" t="n">
-        <v>5.09</v>
+        <v>2.687</v>
       </c>
       <c r="J68" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45164.3923611111</v>
+        <v>45164.4236111111</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -2697,30 +2691,30 @@
         <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E69" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F69" t="n">
-        <v>2.08</v>
+        <v>4.705</v>
       </c>
       <c r="G69" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H69" t="n">
-        <v>1.7</v>
+        <v>1.2185</v>
       </c>
       <c r="I69" t="n">
-        <v>6.9</v>
+        <v>3.322</v>
       </c>
       <c r="J69" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45164.3923611111</v>
+        <v>45164.4236111111</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -2729,25 +2723,25 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F70" t="n">
-        <v>2.1</v>
+        <v>4.705</v>
       </c>
       <c r="G70" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H70" t="n">
-        <v>1.73529411764706</v>
+        <v>1.209</v>
       </c>
       <c r="I70" t="n">
-        <v>5.246</v>
+        <v>3.967</v>
       </c>
       <c r="J70" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71">
@@ -2761,22 +2755,22 @@
         <v>11</v>
       </c>
       <c r="D71" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" t="s">
+        <v>39</v>
+      </c>
+      <c r="F71" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="G71" t="s">
         <v>40</v>
       </c>
-      <c r="E71" t="s">
-        <v>41</v>
-      </c>
-      <c r="F71" t="n">
-        <v>5.085</v>
-      </c>
-      <c r="G71" t="s">
-        <v>42</v>
-      </c>
       <c r="H71" t="n">
-        <v>1.2185</v>
+        <v>1.228</v>
       </c>
       <c r="I71" t="n">
-        <v>1.734</v>
+        <v>3.125</v>
       </c>
       <c r="J71" t="s">
         <v>15</v>
@@ -2793,22 +2787,22 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" t="s">
+        <v>39</v>
+      </c>
+      <c r="F72" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="G72" t="s">
         <v>40</v>
       </c>
-      <c r="E72" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" t="n">
-        <v>5.085</v>
-      </c>
-      <c r="G72" t="s">
-        <v>42</v>
-      </c>
       <c r="H72" t="n">
-        <v>1.209</v>
+        <v>1.2185</v>
       </c>
       <c r="I72" t="n">
-        <v>2.379</v>
+        <v>3.76</v>
       </c>
       <c r="J72" t="s">
         <v>15</v>
@@ -2825,22 +2819,22 @@
         <v>11</v>
       </c>
       <c r="D73" t="s">
+        <v>38</v>
+      </c>
+      <c r="E73" t="s">
+        <v>39</v>
+      </c>
+      <c r="F73" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="G73" t="s">
         <v>40</v>
       </c>
-      <c r="E73" t="s">
-        <v>41</v>
-      </c>
-      <c r="F73" t="n">
-        <v>5.085</v>
-      </c>
-      <c r="G73" t="s">
-        <v>42</v>
-      </c>
       <c r="H73" t="n">
-        <v>1.1995</v>
+        <v>1.209</v>
       </c>
       <c r="I73" t="n">
-        <v>3.034</v>
+        <v>4.405</v>
       </c>
       <c r="J73" t="s">
         <v>15</v>
@@ -2857,22 +2851,22 @@
         <v>11</v>
       </c>
       <c r="D74" t="s">
+        <v>38</v>
+      </c>
+      <c r="E74" t="s">
+        <v>39</v>
+      </c>
+      <c r="F74" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G74" t="s">
         <v>40</v>
       </c>
-      <c r="E74" t="s">
-        <v>41</v>
-      </c>
-      <c r="F74" t="n">
-        <v>5</v>
-      </c>
-      <c r="G74" t="s">
-        <v>42</v>
-      </c>
       <c r="H74" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="I74" t="n">
-        <v>5.47</v>
+        <v>5.556</v>
       </c>
       <c r="J74" t="s">
         <v>16</v>
@@ -2889,16 +2883,16 @@
         <v>11</v>
       </c>
       <c r="D75" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E75" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F75" t="n">
         <v>4.6</v>
       </c>
       <c r="G75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H75" t="n">
         <v>1.2</v>
@@ -2921,22 +2915,22 @@
         <v>11</v>
       </c>
       <c r="D76" t="s">
+        <v>38</v>
+      </c>
+      <c r="E76" t="s">
+        <v>39</v>
+      </c>
+      <c r="F76" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G76" t="s">
         <v>40</v>
       </c>
-      <c r="E76" t="s">
-        <v>41</v>
-      </c>
-      <c r="F76" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G76" t="s">
-        <v>42</v>
-      </c>
       <c r="H76" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="I76" t="n">
-        <v>5.579</v>
+        <v>5.31</v>
       </c>
       <c r="J76" t="s">
         <v>18</v>
@@ -2953,22 +2947,22 @@
         <v>11</v>
       </c>
       <c r="D77" t="s">
+        <v>38</v>
+      </c>
+      <c r="E77" t="s">
+        <v>39</v>
+      </c>
+      <c r="F77" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G77" t="s">
         <v>40</v>
       </c>
-      <c r="E77" t="s">
-        <v>41</v>
-      </c>
-      <c r="F77" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="G77" t="s">
-        <v>42</v>
-      </c>
       <c r="H77" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="I77" t="n">
-        <v>6.485</v>
+        <v>6.256</v>
       </c>
       <c r="J77" t="s">
         <v>19</v>
@@ -2985,22 +2979,22 @@
         <v>11</v>
       </c>
       <c r="D78" t="s">
+        <v>38</v>
+      </c>
+      <c r="E78" t="s">
+        <v>39</v>
+      </c>
+      <c r="F78" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="G78" t="s">
         <v>40</v>
       </c>
-      <c r="E78" t="s">
-        <v>41</v>
-      </c>
-      <c r="F78" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G78" t="s">
-        <v>42</v>
-      </c>
       <c r="H78" t="n">
-        <v>1.2</v>
+        <v>1.22</v>
       </c>
       <c r="I78" t="n">
-        <v>5.556</v>
+        <v>5.497</v>
       </c>
       <c r="J78" t="s">
         <v>20</v>
@@ -3017,22 +3011,22 @@
         <v>11</v>
       </c>
       <c r="D79" t="s">
+        <v>38</v>
+      </c>
+      <c r="E79" t="s">
+        <v>39</v>
+      </c>
+      <c r="F79" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G79" t="s">
         <v>40</v>
       </c>
-      <c r="E79" t="s">
-        <v>41</v>
-      </c>
-      <c r="F79" t="n">
-        <v>5</v>
-      </c>
-      <c r="G79" t="s">
-        <v>42</v>
-      </c>
       <c r="H79" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="I79" t="n">
-        <v>5.47</v>
+        <v>5.556</v>
       </c>
       <c r="J79" t="s">
         <v>21</v>
@@ -3049,22 +3043,22 @@
         <v>11</v>
       </c>
       <c r="D80" t="s">
+        <v>38</v>
+      </c>
+      <c r="E80" t="s">
+        <v>39</v>
+      </c>
+      <c r="F80" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G80" t="s">
         <v>40</v>
       </c>
-      <c r="E80" t="s">
-        <v>41</v>
-      </c>
-      <c r="F80" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="G80" t="s">
-        <v>42</v>
-      </c>
       <c r="H80" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="I80" t="n">
-        <v>5.086</v>
+        <v>5.072</v>
       </c>
       <c r="J80" t="s">
         <v>22</v>
@@ -3081,22 +3075,22 @@
         <v>11</v>
       </c>
       <c r="D81" t="s">
+        <v>38</v>
+      </c>
+      <c r="E81" t="s">
+        <v>39</v>
+      </c>
+      <c r="F81" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G81" t="s">
         <v>40</v>
-      </c>
-      <c r="E81" t="s">
-        <v>41</v>
-      </c>
-      <c r="F81" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G81" t="s">
-        <v>42</v>
       </c>
       <c r="H81" t="n">
         <v>1.2</v>
       </c>
       <c r="I81" t="n">
-        <v>5.556</v>
+        <v>6.061</v>
       </c>
       <c r="J81" t="s">
         <v>23</v>
@@ -3113,30 +3107,30 @@
         <v>11</v>
       </c>
       <c r="D82" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" t="s">
+        <v>39</v>
+      </c>
+      <c r="F82" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G82" t="s">
         <v>40</v>
       </c>
-      <c r="E82" t="s">
-        <v>41</v>
-      </c>
-      <c r="F82" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="G82" t="s">
-        <v>42</v>
-      </c>
       <c r="H82" t="n">
-        <v>1.18867924528302</v>
+        <v>1.2</v>
       </c>
       <c r="I82" t="n">
-        <v>5.18</v>
+        <v>5.556</v>
       </c>
       <c r="J82" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>45165.1041666667</v>
+        <v>45164.4236111111</v>
       </c>
       <c r="B83" t="s">
         <v>10</v>
@@ -3145,25 +3139,25 @@
         <v>11</v>
       </c>
       <c r="D83" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E83" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F83" t="n">
-        <v>1.133</v>
+        <v>4.6</v>
       </c>
       <c r="G83" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H83" t="n">
-        <v>5.655</v>
+        <v>1.18867924528302</v>
       </c>
       <c r="I83" t="n">
-        <v>5.945</v>
+        <v>5.866</v>
       </c>
       <c r="J83" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84">
@@ -3177,22 +3171,22 @@
         <v>11</v>
       </c>
       <c r="D84" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" t="s">
+        <v>42</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1.133</v>
+      </c>
+      <c r="G84" t="s">
         <v>43</v>
       </c>
-      <c r="E84" t="s">
-        <v>44</v>
-      </c>
-      <c r="F84" t="n">
-        <v>1.1235</v>
-      </c>
-      <c r="G84" t="s">
-        <v>45</v>
-      </c>
       <c r="H84" t="n">
-        <v>5.655</v>
+        <v>6.89</v>
       </c>
       <c r="I84" t="n">
-        <v>6.691</v>
+        <v>2.775</v>
       </c>
       <c r="J84" t="s">
         <v>15</v>
@@ -3209,25 +3203,25 @@
         <v>11</v>
       </c>
       <c r="D85" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" t="s">
+        <v>42</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1.1235</v>
+      </c>
+      <c r="G85" t="s">
         <v>43</v>
       </c>
-      <c r="E85" t="s">
-        <v>44</v>
-      </c>
-      <c r="F85" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G85" t="s">
-        <v>45</v>
-      </c>
       <c r="H85" t="n">
-        <v>6.5</v>
+        <v>6.89</v>
       </c>
       <c r="I85" t="n">
-        <v>5.475</v>
+        <v>3.521</v>
       </c>
       <c r="J85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86">
@@ -3241,25 +3235,25 @@
         <v>11</v>
       </c>
       <c r="D86" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" t="s">
+        <v>42</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1.114</v>
+      </c>
+      <c r="G86" t="s">
         <v>43</v>
       </c>
-      <c r="E86" t="s">
-        <v>44</v>
-      </c>
-      <c r="F86" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G86" t="s">
-        <v>45</v>
-      </c>
       <c r="H86" t="n">
-        <v>6.25</v>
+        <v>6.89</v>
       </c>
       <c r="I86" t="n">
-        <v>5.286</v>
+        <v>4.28</v>
       </c>
       <c r="J86" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87">
@@ -3273,25 +3267,25 @@
         <v>11</v>
       </c>
       <c r="D87" t="s">
+        <v>41</v>
+      </c>
+      <c r="E87" t="s">
+        <v>42</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G87" t="s">
         <v>43</v>
       </c>
-      <c r="E87" t="s">
-        <v>44</v>
-      </c>
-      <c r="F87" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G87" t="s">
-        <v>45</v>
-      </c>
       <c r="H87" t="n">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="I87" t="n">
-        <v>5.415</v>
+        <v>5.475</v>
       </c>
       <c r="J87" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88">
@@ -3305,25 +3299,25 @@
         <v>11</v>
       </c>
       <c r="D88" t="s">
+        <v>41</v>
+      </c>
+      <c r="E88" t="s">
+        <v>42</v>
+      </c>
+      <c r="F88" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G88" t="s">
         <v>43</v>
       </c>
-      <c r="E88" t="s">
-        <v>44</v>
-      </c>
-      <c r="F88" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G88" t="s">
-        <v>45</v>
-      </c>
       <c r="H88" t="n">
-        <v>5.9</v>
+        <v>6.25</v>
       </c>
       <c r="I88" t="n">
-        <v>7.039</v>
+        <v>5.286</v>
       </c>
       <c r="J88" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89">
@@ -3337,25 +3331,25 @@
         <v>11</v>
       </c>
       <c r="D89" t="s">
+        <v>41</v>
+      </c>
+      <c r="E89" t="s">
+        <v>42</v>
+      </c>
+      <c r="F89" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G89" t="s">
         <v>43</v>
       </c>
-      <c r="E89" t="s">
-        <v>44</v>
-      </c>
-      <c r="F89" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G89" t="s">
-        <v>45</v>
-      </c>
       <c r="H89" t="n">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="I89" t="n">
-        <v>5.475</v>
+        <v>5.195</v>
       </c>
       <c r="J89" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90">
@@ -3369,25 +3363,25 @@
         <v>11</v>
       </c>
       <c r="D90" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" t="s">
+        <v>42</v>
+      </c>
+      <c r="F90" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G90" t="s">
         <v>43</v>
       </c>
-      <c r="E90" t="s">
-        <v>44</v>
-      </c>
-      <c r="F90" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G90" t="s">
-        <v>45</v>
-      </c>
       <c r="H90" t="n">
-        <v>6.25</v>
+        <v>6.2</v>
       </c>
       <c r="I90" t="n">
-        <v>5.286</v>
+        <v>7.038</v>
       </c>
       <c r="J90" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91">
@@ -3401,25 +3395,25 @@
         <v>11</v>
       </c>
       <c r="D91" t="s">
+        <v>41</v>
+      </c>
+      <c r="E91" t="s">
+        <v>42</v>
+      </c>
+      <c r="F91" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G91" t="s">
         <v>43</v>
       </c>
-      <c r="E91" t="s">
-        <v>44</v>
-      </c>
-      <c r="F91" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G91" t="s">
-        <v>45</v>
-      </c>
       <c r="H91" t="n">
-        <v>6.05</v>
+        <v>6</v>
       </c>
       <c r="I91" t="n">
-        <v>5.025</v>
+        <v>5.952</v>
       </c>
       <c r="J91" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92">
@@ -3433,25 +3427,25 @@
         <v>11</v>
       </c>
       <c r="D92" t="s">
+        <v>41</v>
+      </c>
+      <c r="E92" t="s">
+        <v>42</v>
+      </c>
+      <c r="F92" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G92" t="s">
         <v>43</v>
       </c>
-      <c r="E92" t="s">
-        <v>44</v>
-      </c>
-      <c r="F92" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G92" t="s">
-        <v>45</v>
-      </c>
       <c r="H92" t="n">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="I92" t="n">
-        <v>5.475</v>
+        <v>5.195</v>
       </c>
       <c r="J92" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93">
@@ -3465,25 +3459,25 @@
         <v>11</v>
       </c>
       <c r="D93" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E93" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F93" t="n">
         <v>1.12</v>
       </c>
       <c r="G93" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H93" t="n">
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="I93" t="n">
-        <v>5.952</v>
+        <v>5.286</v>
       </c>
       <c r="J93" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
@@ -3497,30 +3491,30 @@
         <v>11</v>
       </c>
       <c r="D94" t="s">
+        <v>41</v>
+      </c>
+      <c r="E94" t="s">
+        <v>42</v>
+      </c>
+      <c r="F94" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G94" t="s">
         <v>43</v>
       </c>
-      <c r="E94" t="s">
-        <v>44</v>
-      </c>
-      <c r="F94" t="n">
-        <v>1.11976047904192</v>
-      </c>
-      <c r="G94" t="s">
-        <v>45</v>
-      </c>
       <c r="H94" t="n">
-        <v>6.25</v>
+        <v>5.75</v>
       </c>
       <c r="I94" t="n">
-        <v>5.305</v>
+        <v>5.887</v>
       </c>
       <c r="J94" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.1041666667</v>
       </c>
       <c r="B95" t="s">
         <v>10</v>
@@ -3529,30 +3523,30 @@
         <v>11</v>
       </c>
       <c r="D95" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E95" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F95" t="n">
-        <v>1.8</v>
+        <v>1.1</v>
       </c>
       <c r="G95" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H95" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I95" t="n">
-        <v>5.556</v>
+        <v>5.195</v>
       </c>
       <c r="J95" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.1041666667</v>
       </c>
       <c r="B96" t="s">
         <v>10</v>
@@ -3561,30 +3555,30 @@
         <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E96" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F96" t="n">
-        <v>1.8</v>
+        <v>1.1</v>
       </c>
       <c r="G96" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H96" t="n">
-        <v>2.02</v>
+        <v>7</v>
       </c>
       <c r="I96" t="n">
-        <v>5.061</v>
+        <v>5.195</v>
       </c>
       <c r="J96" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>45165.2222222222</v>
+        <v>45165.1041666667</v>
       </c>
       <c r="B97" t="s">
         <v>10</v>
@@ -3593,25 +3587,25 @@
         <v>11</v>
       </c>
       <c r="D97" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E97" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F97" t="n">
-        <v>1.8</v>
+        <v>1.1</v>
       </c>
       <c r="G97" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H97" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I97" t="n">
-        <v>5.556</v>
+        <v>5.195</v>
       </c>
       <c r="J97" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98">
@@ -3625,25 +3619,25 @@
         <v>11</v>
       </c>
       <c r="D98" t="s">
+        <v>44</v>
+      </c>
+      <c r="E98" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1.8455</v>
+      </c>
+      <c r="G98" t="s">
         <v>46</v>
       </c>
-      <c r="E98" t="s">
-        <v>47</v>
-      </c>
-      <c r="F98" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="G98" t="s">
-        <v>48</v>
-      </c>
       <c r="H98" t="n">
-        <v>2</v>
+        <v>2.045</v>
       </c>
       <c r="I98" t="n">
-        <v>6.18</v>
+        <v>3.086</v>
       </c>
       <c r="J98" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99">
@@ -3657,25 +3651,25 @@
         <v>11</v>
       </c>
       <c r="D99" t="s">
+        <v>44</v>
+      </c>
+      <c r="E99" t="s">
+        <v>45</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1.8455</v>
+      </c>
+      <c r="G99" t="s">
         <v>46</v>
       </c>
-      <c r="E99" t="s">
-        <v>47</v>
-      </c>
-      <c r="F99" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G99" t="s">
-        <v>48</v>
-      </c>
       <c r="H99" t="n">
-        <v>2</v>
+        <v>2.026</v>
       </c>
       <c r="I99" t="n">
-        <v>5.556</v>
+        <v>3.544</v>
       </c>
       <c r="J99" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100">
@@ -3689,25 +3683,25 @@
         <v>11</v>
       </c>
       <c r="D100" t="s">
+        <v>44</v>
+      </c>
+      <c r="E100" t="s">
+        <v>45</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1.8455</v>
+      </c>
+      <c r="G100" t="s">
         <v>46</v>
       </c>
-      <c r="E100" t="s">
-        <v>47</v>
-      </c>
-      <c r="F100" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="G100" t="s">
-        <v>48</v>
-      </c>
       <c r="H100" t="n">
-        <v>2.08</v>
+        <v>2.007</v>
       </c>
       <c r="I100" t="n">
-        <v>5.22</v>
+        <v>4.011</v>
       </c>
       <c r="J100" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101">
@@ -3721,25 +3715,25 @@
         <v>11</v>
       </c>
       <c r="D101" t="s">
+        <v>44</v>
+      </c>
+      <c r="E101" t="s">
+        <v>45</v>
+      </c>
+      <c r="F101" t="n">
+        <v>1.836</v>
+      </c>
+      <c r="G101" t="s">
         <v>46</v>
       </c>
-      <c r="E101" t="s">
-        <v>47</v>
-      </c>
-      <c r="F101" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="G101" t="s">
-        <v>48</v>
-      </c>
       <c r="H101" t="n">
-        <v>2.04</v>
+        <v>2.045</v>
       </c>
       <c r="I101" t="n">
-        <v>4.268</v>
+        <v>3.366</v>
       </c>
       <c r="J101" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102">
@@ -3753,25 +3747,25 @@
         <v>11</v>
       </c>
       <c r="D102" t="s">
+        <v>44</v>
+      </c>
+      <c r="E102" t="s">
+        <v>45</v>
+      </c>
+      <c r="F102" t="n">
+        <v>1.836</v>
+      </c>
+      <c r="G102" t="s">
         <v>46</v>
       </c>
-      <c r="E102" t="s">
-        <v>47</v>
-      </c>
-      <c r="F102" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G102" t="s">
-        <v>48</v>
-      </c>
       <c r="H102" t="n">
-        <v>2</v>
+        <v>2.026</v>
       </c>
       <c r="I102" t="n">
-        <v>5.556</v>
+        <v>3.825</v>
       </c>
       <c r="J102" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103">
@@ -3785,25 +3779,25 @@
         <v>11</v>
       </c>
       <c r="D103" t="s">
+        <v>44</v>
+      </c>
+      <c r="E103" t="s">
+        <v>45</v>
+      </c>
+      <c r="F103" t="n">
+        <v>1.836</v>
+      </c>
+      <c r="G103" t="s">
         <v>46</v>
       </c>
-      <c r="E103" t="s">
-        <v>47</v>
-      </c>
-      <c r="F103" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="G103" t="s">
-        <v>48</v>
-      </c>
       <c r="H103" t="n">
-        <v>2</v>
+        <v>2.007</v>
       </c>
       <c r="I103" t="n">
-        <v>6.18</v>
+        <v>4.292</v>
       </c>
       <c r="J103" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104">
@@ -3817,30 +3811,30 @@
         <v>11</v>
       </c>
       <c r="D104" t="s">
+        <v>44</v>
+      </c>
+      <c r="E104" t="s">
+        <v>45</v>
+      </c>
+      <c r="F104" t="n">
+        <v>1.8265</v>
+      </c>
+      <c r="G104" t="s">
         <v>46</v>
       </c>
-      <c r="E104" t="s">
-        <v>47</v>
-      </c>
-      <c r="F104" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="G104" t="s">
-        <v>48</v>
-      </c>
       <c r="H104" t="n">
-        <v>2.02</v>
+        <v>2.045</v>
       </c>
       <c r="I104" t="n">
-        <v>5.061</v>
+        <v>3.649</v>
       </c>
       <c r="J104" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
@@ -3849,30 +3843,30 @@
         <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E105" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F105" t="n">
-        <v>1.5</v>
+        <v>1.8265</v>
       </c>
       <c r="G105" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H105" t="n">
-        <v>2.6</v>
+        <v>2.026</v>
       </c>
       <c r="I105" t="n">
-        <v>5.128</v>
+        <v>4.108</v>
       </c>
       <c r="J105" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B106" t="s">
         <v>10</v>
@@ -3881,30 +3875,30 @@
         <v>11</v>
       </c>
       <c r="D106" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E106" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F106" t="n">
-        <v>1.52</v>
+        <v>1.8265</v>
       </c>
       <c r="G106" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H106" t="n">
-        <v>2.55</v>
+        <v>2.007</v>
       </c>
       <c r="I106" t="n">
-        <v>5.005</v>
+        <v>4.575</v>
       </c>
       <c r="J106" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B107" t="s">
         <v>10</v>
@@ -3913,30 +3907,30 @@
         <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E107" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F107" t="n">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G107" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H107" t="n">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="I107" t="n">
-        <v>5.128</v>
+        <v>5.556</v>
       </c>
       <c r="J107" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B108" t="s">
         <v>10</v>
@@ -3945,30 +3939,30 @@
         <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E108" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F108" t="n">
-        <v>1.5</v>
+        <v>1.77</v>
       </c>
       <c r="G108" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H108" t="n">
-        <v>2.5</v>
+        <v>2.05</v>
       </c>
       <c r="I108" t="n">
-        <v>6.667</v>
+        <v>5.278</v>
       </c>
       <c r="J108" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B109" t="s">
         <v>10</v>
@@ -3977,30 +3971,30 @@
         <v>11</v>
       </c>
       <c r="D109" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E109" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F109" t="n">
-        <v>1.53</v>
+        <v>1.8</v>
       </c>
       <c r="G109" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H109" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="I109" t="n">
-        <v>5.359</v>
+        <v>5.556</v>
       </c>
       <c r="J109" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B110" t="s">
         <v>10</v>
@@ -4009,30 +4003,30 @@
         <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E110" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F110" t="n">
-        <v>1.52</v>
+        <v>1.73</v>
       </c>
       <c r="G110" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H110" t="n">
-        <v>2.54</v>
+        <v>2.06</v>
       </c>
       <c r="I110" t="n">
-        <v>5.16</v>
+        <v>6.347</v>
       </c>
       <c r="J110" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -4041,30 +4035,30 @@
         <v>11</v>
       </c>
       <c r="D111" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E111" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F111" t="n">
-        <v>1.52</v>
+        <v>1.8</v>
       </c>
       <c r="G111" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H111" t="n">
-        <v>2.55</v>
+        <v>2.02</v>
       </c>
       <c r="I111" t="n">
-        <v>5.005</v>
+        <v>5.061</v>
       </c>
       <c r="J111" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>45165.3402777778</v>
+        <v>45165.2222222222</v>
       </c>
       <c r="B112" t="s">
         <v>10</v>
@@ -4073,57 +4067,505 @@
         <v>11</v>
       </c>
       <c r="D112" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E112" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F112" t="n">
-        <v>1.5</v>
+        <v>1.77</v>
       </c>
       <c r="G112" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H112" t="n">
-        <v>2.5</v>
+        <v>2.05</v>
       </c>
       <c r="I112" t="n">
-        <v>6.667</v>
+        <v>5.278</v>
       </c>
       <c r="J112" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
+        <v>45165.2222222222</v>
+      </c>
+      <c r="B113" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" t="s">
+        <v>44</v>
+      </c>
+      <c r="E113" t="s">
+        <v>45</v>
+      </c>
+      <c r="F113" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G113" t="s">
+        <v>46</v>
+      </c>
+      <c r="H113" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I113" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J113" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>45165.2222222222</v>
+      </c>
+      <c r="B114" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" t="s">
+        <v>44</v>
+      </c>
+      <c r="E114" t="s">
+        <v>45</v>
+      </c>
+      <c r="F114" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G114" t="s">
+        <v>46</v>
+      </c>
+      <c r="H114" t="n">
+        <v>2</v>
+      </c>
+      <c r="I114" t="n">
+        <v>5.556</v>
+      </c>
+      <c r="J114" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>45165.2222222222</v>
+      </c>
+      <c r="B115" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" t="s">
+        <v>44</v>
+      </c>
+      <c r="E115" t="s">
+        <v>45</v>
+      </c>
+      <c r="F115" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G115" t="s">
+        <v>46</v>
+      </c>
+      <c r="H115" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I115" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J115" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>45165.2222222222</v>
+      </c>
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" t="s">
+        <v>44</v>
+      </c>
+      <c r="E116" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G116" t="s">
+        <v>46</v>
+      </c>
+      <c r="H116" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="I116" t="n">
+        <v>5.335</v>
+      </c>
+      <c r="J116" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>45165.2222222222</v>
+      </c>
+      <c r="B117" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" t="s">
+        <v>44</v>
+      </c>
+      <c r="E117" t="s">
+        <v>45</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G117" t="s">
+        <v>46</v>
+      </c>
+      <c r="H117" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="I117" t="n">
+        <v>5.061</v>
+      </c>
+      <c r="J117" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
         <v>45165.3402777778</v>
       </c>
-      <c r="B113" t="s">
-        <v>10</v>
-      </c>
-      <c r="C113" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="B118" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" t="s">
+        <v>47</v>
+      </c>
+      <c r="E118" t="s">
+        <v>48</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G118" t="s">
         <v>49</v>
       </c>
-      <c r="E113" t="s">
+      <c r="H118" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I118" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J118" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B119" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" t="s">
+        <v>47</v>
+      </c>
+      <c r="E119" t="s">
+        <v>48</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G119" t="s">
+        <v>49</v>
+      </c>
+      <c r="H119" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I119" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J119" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B120" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" t="s">
+        <v>47</v>
+      </c>
+      <c r="E120" t="s">
+        <v>48</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G120" t="s">
+        <v>49</v>
+      </c>
+      <c r="H120" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I120" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="J120" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B121" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" t="s">
+        <v>47</v>
+      </c>
+      <c r="E121" t="s">
+        <v>48</v>
+      </c>
+      <c r="F121" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G121" t="s">
+        <v>49</v>
+      </c>
+      <c r="H121" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="I121" t="n">
+        <v>6.347</v>
+      </c>
+      <c r="J121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B122" t="s">
+        <v>10</v>
+      </c>
+      <c r="C122" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" t="s">
+        <v>47</v>
+      </c>
+      <c r="E122" t="s">
+        <v>48</v>
+      </c>
+      <c r="F122" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G122" t="s">
+        <v>49</v>
+      </c>
+      <c r="H122" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I122" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J122" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B123" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" t="s">
+        <v>47</v>
+      </c>
+      <c r="E123" t="s">
+        <v>48</v>
+      </c>
+      <c r="F123" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G123" t="s">
+        <v>49</v>
+      </c>
+      <c r="H123" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I123" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J123" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" t="s">
+        <v>47</v>
+      </c>
+      <c r="E124" t="s">
+        <v>48</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G124" t="s">
+        <v>49</v>
+      </c>
+      <c r="H124" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="I124" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="J124" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B125" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>47</v>
+      </c>
+      <c r="E125" t="s">
+        <v>48</v>
+      </c>
+      <c r="F125" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G125" t="s">
         <v>50</v>
       </c>
-      <c r="F113" t="n">
-        <v>1.51282051282051</v>
-      </c>
-      <c r="G113" t="s">
-        <v>51</v>
-      </c>
-      <c r="H113" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="I113" t="n">
-        <v>5.317</v>
-      </c>
-      <c r="J113" t="s">
+      <c r="H125" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I125" t="n">
+        <v>5.278</v>
+      </c>
+      <c r="J125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B126" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>47</v>
+      </c>
+      <c r="E126" t="s">
+        <v>48</v>
+      </c>
+      <c r="F126" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G126" t="s">
+        <v>49</v>
+      </c>
+      <c r="H126" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="I126" t="n">
+        <v>5.548</v>
+      </c>
+      <c r="J126" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>45165.3402777778</v>
+      </c>
+      <c r="B127" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" t="s">
+        <v>47</v>
+      </c>
+      <c r="E127" t="s">
+        <v>48</v>
+      </c>
+      <c r="F127" t="n">
+        <v>1.6993006993007</v>
+      </c>
+      <c r="G127" t="s">
+        <v>49</v>
+      </c>
+      <c r="H127" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="I127" t="n">
+        <v>4.931</v>
+      </c>
+      <c r="J127" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>